<commit_message>
[Feat] (Client) Create SetExcelStat Function In Monster Class Which Set Moster Stats Based On Excel Loaded Info
</commit_message>
<xml_diff>
--- a/CharacterStats.xlsx
+++ b/CharacterStats.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="79" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="79" uniqueCount="41">
   <si>
     <t>Created by LibXL trial version 4.0.3. Please buy the LibXL full version for removing this message.</t>
   </si>
@@ -72,28 +72,25 @@
     <t>Normal</t>
   </si>
   <si>
-    <t>TRUE</t>
+    <t>FALSE</t>
+  </si>
+  <si>
+    <t>Chicken</t>
   </si>
   <si>
     <t>YellowBird</t>
   </si>
   <si>
-    <t>FALSE</t>
-  </si>
-  <si>
-    <t>Chicken</t>
+    <t>Frog</t>
   </si>
   <si>
     <t>MushRoom</t>
   </si>
   <si>
-    <t>Frog</t>
+    <t>Kabu</t>
   </si>
   <si>
     <t>PurpleBeatle</t>
-  </si>
-  <si>
-    <t>Kabu</t>
   </si>
   <si>
     <t>NormalBear</t>
@@ -712,7 +709,7 @@
         <v>100</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H10" s="5">
         <v>50</v>
@@ -729,7 +726,7 @@
     </row>
     <row r="11" ht="28" customHeight="true" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>18</v>
@@ -747,7 +744,7 @@
         <v>100</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H11" s="5">
         <v>50</v>
@@ -764,7 +761,7 @@
     </row>
     <row r="12" ht="28" customHeight="true" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>18</v>
@@ -799,7 +796,7 @@
     </row>
     <row r="13" ht="28" customHeight="true" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>18</v>
@@ -834,7 +831,7 @@
     </row>
     <row r="14" ht="28" customHeight="true" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>18</v>
@@ -852,13 +849,13 @@
         <v>100</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H14" s="5">
         <v>50</v>
       </c>
       <c r="I14" s="5">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="J14" s="5">
         <v>0</v>
@@ -869,7 +866,7 @@
     </row>
     <row r="15" ht="28" customHeight="true" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>18</v>
@@ -893,7 +890,7 @@
         <v>50</v>
       </c>
       <c r="I15" s="5">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="J15" s="5">
         <v>0</v>
@@ -904,7 +901,7 @@
     </row>
     <row r="16" ht="28" customHeight="true" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>18</v>
@@ -939,10 +936,10 @@
     </row>
     <row r="17" ht="28" customHeight="true" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17" s="5" t="s">
         <v>28</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>29</v>
       </c>
       <c r="C17" s="5">
         <v>100</v>
@@ -957,7 +954,7 @@
         <v>100</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H17" s="5">
         <v>50</v>
@@ -974,10 +971,10 @@
     </row>
     <row r="18" ht="28" customHeight="true" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C18" s="5">
         <v>100</v>
@@ -992,7 +989,7 @@
         <v>100</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H18" s="5">
         <v>50</v>
@@ -1009,10 +1006,10 @@
     </row>
     <row r="19" ht="28" customHeight="true" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B19" s="5" t="s">
         <v>31</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>32</v>
       </c>
       <c r="C19" s="5">
         <v>300</v>
@@ -1041,15 +1038,15 @@
       <c r="K19" s="5"/>
       <c r="L19" s="5"/>
       <c r="M19" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="20" ht="28" customHeight="true" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C20" s="5">
         <v>300</v>
@@ -1078,15 +1075,15 @@
       <c r="K20" s="5"/>
       <c r="L20" s="5"/>
       <c r="M20" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="21" ht="28" customHeight="true" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C21" s="5">
         <v>300</v>
@@ -1115,15 +1112,15 @@
       <c r="K21" s="5"/>
       <c r="L21" s="5"/>
       <c r="M21" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="22" ht="28" customHeight="true" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C22" s="5">
         <v>300</v>
@@ -1152,15 +1149,15 @@
       <c r="K22" s="5"/>
       <c r="L22" s="5"/>
       <c r="M22" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="23" ht="28" customHeight="true" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C23" s="5">
         <v>300</v>
@@ -1189,15 +1186,15 @@
       <c r="K23" s="5"/>
       <c r="L23" s="5"/>
       <c r="M23" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="24" ht="28" customHeight="true" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B24" s="5" t="s">
         <v>37</v>
-      </c>
-      <c r="B24" s="5" t="s">
-        <v>38</v>
       </c>
       <c r="C24" s="5">
         <v>5000</v>
@@ -1233,10 +1230,10 @@
     </row>
     <row r="25" ht="28" customHeight="true" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C25" s="5">
         <v>5000</v>
@@ -1251,7 +1248,7 @@
         <v>100</v>
       </c>
       <c r="G25" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H25" s="5">
         <v>150</v>
@@ -1272,10 +1269,10 @@
     </row>
     <row r="26" ht="28" customHeight="true" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C26" s="5">
         <v>3000</v>
@@ -1311,10 +1308,10 @@
     </row>
     <row r="27" ht="28" customHeight="true" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C27" s="5">
         <v>3000</v>

</xml_diff>

<commit_message>
[Feat] (Client) Decrease MP When Player Special Attack , FallDownAttack, GoUpAttack
</commit_message>
<xml_diff>
--- a/CharacterStats.xlsx
+++ b/CharacterStats.xlsx
@@ -75,22 +75,22 @@
     <t>FALSE</t>
   </si>
   <si>
+    <t>YellowBird</t>
+  </si>
+  <si>
     <t>Chicken</t>
   </si>
   <si>
-    <t>YellowBird</t>
+    <t>MushRoom</t>
   </si>
   <si>
     <t>Frog</t>
   </si>
   <si>
-    <t>MushRoom</t>
+    <t>PurpleBeatle</t>
   </si>
   <si>
     <t>Kabu</t>
-  </si>
-  <si>
-    <t>PurpleBeatle</t>
   </si>
   <si>
     <t>NormalBear</t>
@@ -855,7 +855,7 @@
         <v>50</v>
       </c>
       <c r="I14" s="5">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="J14" s="5">
         <v>0</v>
@@ -890,7 +890,7 @@
         <v>50</v>
       </c>
       <c r="I15" s="5">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="J15" s="5">
         <v>0</v>
@@ -945,10 +945,10 @@
         <v>100</v>
       </c>
       <c r="D17" s="5">
-        <v>65</v>
+        <v>550</v>
       </c>
       <c r="E17" s="5">
-        <v>550</v>
+        <v>200</v>
       </c>
       <c r="F17" s="5">
         <v>100</v>
@@ -980,10 +980,10 @@
         <v>100</v>
       </c>
       <c r="D18" s="5">
-        <v>65</v>
+        <v>550</v>
       </c>
       <c r="E18" s="5">
-        <v>550</v>
+        <v>200</v>
       </c>
       <c r="F18" s="5">
         <v>100</v>
@@ -1299,7 +1299,7 @@
         <v>60</v>
       </c>
       <c r="K26" s="5">
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="L26" s="5">
         <v>600</v>

</xml_diff>

<commit_message>
[Fix] (Client) Use sheet->writeBool Function When Write m_IsGroundObject Info Of MonsterStat To Excel File
</commit_message>
<xml_diff>
--- a/CharacterStats.xlsx
+++ b/CharacterStats.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="79" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="60" uniqueCount="40">
   <si>
     <t>Created by LibXL trial version 4.0.3. Please buy the LibXL full version for removing this message.</t>
   </si>
@@ -70,9 +70,6 @@
   </si>
   <si>
     <t>Normal</t>
-  </si>
-  <si>
-    <t>FALSE</t>
   </si>
   <si>
     <t>YellowBird</t>
@@ -673,8 +670,8 @@
       <c r="F9" s="5">
         <v>100</v>
       </c>
-      <c r="G9" s="5" t="s">
-        <v>19</v>
+      <c r="G9" s="5" t="b">
+        <v>1</v>
       </c>
       <c r="H9" s="5">
         <v>50</v>
@@ -691,7 +688,7 @@
     </row>
     <row r="10" ht="28" customHeight="true" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>18</v>
@@ -708,8 +705,8 @@
       <c r="F10" s="5">
         <v>100</v>
       </c>
-      <c r="G10" s="5" t="s">
-        <v>19</v>
+      <c r="G10" s="5" t="b">
+        <v>0</v>
       </c>
       <c r="H10" s="5">
         <v>50</v>
@@ -726,7 +723,7 @@
     </row>
     <row r="11" ht="28" customHeight="true" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>18</v>
@@ -743,8 +740,8 @@
       <c r="F11" s="5">
         <v>100</v>
       </c>
-      <c r="G11" s="5" t="s">
-        <v>19</v>
+      <c r="G11" s="5" t="b">
+        <v>0</v>
       </c>
       <c r="H11" s="5">
         <v>50</v>
@@ -761,7 +758,7 @@
     </row>
     <row r="12" ht="28" customHeight="true" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>18</v>
@@ -778,8 +775,8 @@
       <c r="F12" s="5">
         <v>100</v>
       </c>
-      <c r="G12" s="5" t="s">
-        <v>19</v>
+      <c r="G12" s="5" t="b">
+        <v>1</v>
       </c>
       <c r="H12" s="5">
         <v>50</v>
@@ -796,7 +793,7 @@
     </row>
     <row r="13" ht="28" customHeight="true" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>18</v>
@@ -813,8 +810,8 @@
       <c r="F13" s="5">
         <v>100</v>
       </c>
-      <c r="G13" s="5" t="s">
-        <v>19</v>
+      <c r="G13" s="5" t="b">
+        <v>1</v>
       </c>
       <c r="H13" s="5">
         <v>50</v>
@@ -831,7 +828,7 @@
     </row>
     <row r="14" ht="28" customHeight="true" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>18</v>
@@ -848,8 +845,8 @@
       <c r="F14" s="5">
         <v>100</v>
       </c>
-      <c r="G14" s="5" t="s">
-        <v>19</v>
+      <c r="G14" s="5" t="b">
+        <v>0</v>
       </c>
       <c r="H14" s="5">
         <v>50</v>
@@ -866,7 +863,7 @@
     </row>
     <row r="15" ht="28" customHeight="true" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>18</v>
@@ -883,8 +880,8 @@
       <c r="F15" s="5">
         <v>100</v>
       </c>
-      <c r="G15" s="5" t="s">
-        <v>19</v>
+      <c r="G15" s="5" t="b">
+        <v>1</v>
       </c>
       <c r="H15" s="5">
         <v>50</v>
@@ -901,7 +898,7 @@
     </row>
     <row r="16" ht="28" customHeight="true" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>18</v>
@@ -918,8 +915,8 @@
       <c r="F16" s="5">
         <v>150</v>
       </c>
-      <c r="G16" s="5" t="s">
-        <v>19</v>
+      <c r="G16" s="5" t="b">
+        <v>1</v>
       </c>
       <c r="H16" s="5">
         <v>80</v>
@@ -936,25 +933,25 @@
     </row>
     <row r="17" ht="28" customHeight="true" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B17" s="5" t="s">
-        <v>28</v>
-      </c>
       <c r="C17" s="5">
         <v>100</v>
       </c>
       <c r="D17" s="5">
+        <v>65</v>
+      </c>
+      <c r="E17" s="5">
         <v>550</v>
       </c>
-      <c r="E17" s="5">
-        <v>200</v>
-      </c>
       <c r="F17" s="5">
         <v>100</v>
       </c>
-      <c r="G17" s="5" t="s">
-        <v>19</v>
+      <c r="G17" s="5" t="b">
+        <v>0</v>
       </c>
       <c r="H17" s="5">
         <v>50</v>
@@ -971,25 +968,25 @@
     </row>
     <row r="18" ht="28" customHeight="true" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C18" s="5">
         <v>100</v>
       </c>
       <c r="D18" s="5">
+        <v>65</v>
+      </c>
+      <c r="E18" s="5">
         <v>550</v>
       </c>
-      <c r="E18" s="5">
-        <v>200</v>
-      </c>
       <c r="F18" s="5">
         <v>100</v>
       </c>
-      <c r="G18" s="5" t="s">
-        <v>19</v>
+      <c r="G18" s="5" t="b">
+        <v>0</v>
       </c>
       <c r="H18" s="5">
         <v>50</v>
@@ -1006,10 +1003,10 @@
     </row>
     <row r="19" ht="28" customHeight="true" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B19" s="5" t="s">
         <v>30</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>31</v>
       </c>
       <c r="C19" s="5">
         <v>300</v>
@@ -1023,8 +1020,8 @@
       <c r="F19" s="5">
         <v>100</v>
       </c>
-      <c r="G19" s="5" t="s">
-        <v>19</v>
+      <c r="G19" s="5" t="b">
+        <v>1</v>
       </c>
       <c r="H19" s="5">
         <v>100</v>
@@ -1038,15 +1035,15 @@
       <c r="K19" s="5"/>
       <c r="L19" s="5"/>
       <c r="M19" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="20" ht="28" customHeight="true" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C20" s="5">
         <v>300</v>
@@ -1060,8 +1057,8 @@
       <c r="F20" s="5">
         <v>100</v>
       </c>
-      <c r="G20" s="5" t="s">
-        <v>19</v>
+      <c r="G20" s="5" t="b">
+        <v>1</v>
       </c>
       <c r="H20" s="5">
         <v>150</v>
@@ -1075,15 +1072,15 @@
       <c r="K20" s="5"/>
       <c r="L20" s="5"/>
       <c r="M20" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="21" ht="28" customHeight="true" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C21" s="5">
         <v>300</v>
@@ -1097,8 +1094,8 @@
       <c r="F21" s="5">
         <v>100</v>
       </c>
-      <c r="G21" s="5" t="s">
-        <v>19</v>
+      <c r="G21" s="5" t="b">
+        <v>1</v>
       </c>
       <c r="H21" s="5">
         <v>150</v>
@@ -1112,15 +1109,15 @@
       <c r="K21" s="5"/>
       <c r="L21" s="5"/>
       <c r="M21" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="22" ht="28" customHeight="true" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C22" s="5">
         <v>300</v>
@@ -1134,8 +1131,8 @@
       <c r="F22" s="5">
         <v>100</v>
       </c>
-      <c r="G22" s="5" t="s">
-        <v>19</v>
+      <c r="G22" s="5" t="b">
+        <v>1</v>
       </c>
       <c r="H22" s="5">
         <v>150</v>
@@ -1149,15 +1146,15 @@
       <c r="K22" s="5"/>
       <c r="L22" s="5"/>
       <c r="M22" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="23" ht="28" customHeight="true" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C23" s="5">
         <v>300</v>
@@ -1171,8 +1168,8 @@
       <c r="F23" s="5">
         <v>100</v>
       </c>
-      <c r="G23" s="5" t="s">
-        <v>19</v>
+      <c r="G23" s="5" t="b">
+        <v>1</v>
       </c>
       <c r="H23" s="5">
         <v>150</v>
@@ -1186,15 +1183,15 @@
       <c r="K23" s="5"/>
       <c r="L23" s="5"/>
       <c r="M23" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="24" ht="28" customHeight="true" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B24" s="5" t="s">
         <v>36</v>
-      </c>
-      <c r="B24" s="5" t="s">
-        <v>37</v>
       </c>
       <c r="C24" s="5">
         <v>5000</v>
@@ -1208,8 +1205,8 @@
       <c r="F24" s="5">
         <v>200</v>
       </c>
-      <c r="G24" s="5" t="s">
-        <v>19</v>
+      <c r="G24" s="5" t="b">
+        <v>1</v>
       </c>
       <c r="H24" s="5">
         <v>150</v>
@@ -1230,10 +1227,10 @@
     </row>
     <row r="25" ht="28" customHeight="true" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C25" s="5">
         <v>5000</v>
@@ -1247,8 +1244,8 @@
       <c r="F25" s="5">
         <v>100</v>
       </c>
-      <c r="G25" s="5" t="s">
-        <v>19</v>
+      <c r="G25" s="5" t="b">
+        <v>0</v>
       </c>
       <c r="H25" s="5">
         <v>150</v>
@@ -1269,10 +1266,10 @@
     </row>
     <row r="26" ht="28" customHeight="true" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C26" s="5">
         <v>3000</v>
@@ -1286,8 +1283,8 @@
       <c r="F26" s="5">
         <v>150</v>
       </c>
-      <c r="G26" s="5" t="s">
-        <v>19</v>
+      <c r="G26" s="5" t="b">
+        <v>1</v>
       </c>
       <c r="H26" s="5">
         <v>100</v>
@@ -1299,7 +1296,7 @@
         <v>60</v>
       </c>
       <c r="K26" s="5">
-        <v>0</v>
+        <v>250</v>
       </c>
       <c r="L26" s="5">
         <v>600</v>
@@ -1308,10 +1305,10 @@
     </row>
     <row r="27" ht="28" customHeight="true" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C27" s="5">
         <v>3000</v>
@@ -1325,8 +1322,8 @@
       <c r="F27" s="5">
         <v>100</v>
       </c>
-      <c r="G27" s="5" t="s">
-        <v>19</v>
+      <c r="G27" s="5" t="b">
+        <v>1</v>
       </c>
       <c r="H27" s="5">
         <v>100</v>

</xml_diff>

<commit_message>
[Feat] (Client) Prevent Player Special Attack When Player Is Flying
</commit_message>
<xml_diff>
--- a/CharacterStats.xlsx
+++ b/CharacterStats.xlsx
@@ -72,22 +72,22 @@
     <t>Normal</t>
   </si>
   <si>
+    <t>Chicken</t>
+  </si>
+  <si>
     <t>YellowBird</t>
   </si>
   <si>
-    <t>Chicken</t>
+    <t>Frog</t>
   </si>
   <si>
     <t>MushRoom</t>
   </si>
   <si>
-    <t>Frog</t>
+    <t>Kabu</t>
   </si>
   <si>
     <t>PurpleBeatle</t>
-  </si>
-  <si>
-    <t>Kabu</t>
   </si>
   <si>
     <t>NormalBear</t>
@@ -846,13 +846,13 @@
         <v>100</v>
       </c>
       <c r="G14" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H14" s="5">
         <v>50</v>
       </c>
       <c r="I14" s="5">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="J14" s="5">
         <v>0</v>
@@ -881,13 +881,13 @@
         <v>100</v>
       </c>
       <c r="G15" s="5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H15" s="5">
         <v>50</v>
       </c>
       <c r="I15" s="5">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="J15" s="5">
         <v>0</v>

</xml_diff>

<commit_message>
[Feat] (Client) Decrease Opacity Of BossHUD After Boss Monster Is Dead
</commit_message>
<xml_diff>
--- a/CharacterStats.xlsx
+++ b/CharacterStats.xlsx
@@ -72,22 +72,22 @@
     <t>Normal</t>
   </si>
   <si>
+    <t>YellowBird</t>
+  </si>
+  <si>
     <t>Chicken</t>
   </si>
   <si>
-    <t>YellowBird</t>
+    <t>MushRoom</t>
   </si>
   <si>
     <t>Frog</t>
   </si>
   <si>
-    <t>MushRoom</t>
+    <t>PurpleBeatle</t>
   </si>
   <si>
     <t>Kabu</t>
-  </si>
-  <si>
-    <t>PurpleBeatle</t>
   </si>
   <si>
     <t>NormalBear</t>
@@ -846,13 +846,13 @@
         <v>100</v>
       </c>
       <c r="G14" s="5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H14" s="5">
         <v>50</v>
       </c>
       <c r="I14" s="5">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="J14" s="5">
         <v>0</v>
@@ -881,13 +881,13 @@
         <v>100</v>
       </c>
       <c r="G15" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H15" s="5">
         <v>50</v>
       </c>
       <c r="I15" s="5">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="J15" s="5">
         <v>0</v>

</xml_diff>

<commit_message>
[Feat] (Client) Add m_DestroyWhenCollide Variiable To KirbyAttackEffect Class & Destroy AttackEffect When It Is True
</commit_message>
<xml_diff>
--- a/CharacterStats.xlsx
+++ b/CharacterStats.xlsx
@@ -72,22 +72,22 @@
     <t>Normal</t>
   </si>
   <si>
+    <t>Chicken</t>
+  </si>
+  <si>
     <t>YellowBird</t>
   </si>
   <si>
-    <t>Chicken</t>
+    <t>Frog</t>
   </si>
   <si>
     <t>MushRoom</t>
   </si>
   <si>
-    <t>Frog</t>
+    <t>Kabu</t>
   </si>
   <si>
     <t>PurpleBeatle</t>
-  </si>
-  <si>
-    <t>Kabu</t>
   </si>
   <si>
     <t>NormalBear</t>
@@ -846,13 +846,13 @@
         <v>100</v>
       </c>
       <c r="G14" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H14" s="5">
         <v>50</v>
       </c>
       <c r="I14" s="5">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="J14" s="5">
         <v>0</v>
@@ -881,13 +881,13 @@
         <v>100</v>
       </c>
       <c r="G15" s="5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H15" s="5">
         <v>50</v>
       </c>
       <c r="I15" s="5">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="J15" s="5">
         <v>0</v>

</xml_diff>

<commit_message>
[Fix] (Client) Block Destroy When PlayerAttack Collider & Do Not Destroy When Player Collide
</commit_message>
<xml_diff>
--- a/CharacterStats.xlsx
+++ b/CharacterStats.xlsx
@@ -72,22 +72,22 @@
     <t>Normal</t>
   </si>
   <si>
+    <t>YellowBird</t>
+  </si>
+  <si>
     <t>Chicken</t>
   </si>
   <si>
-    <t>YellowBird</t>
+    <t>MushRoom</t>
   </si>
   <si>
     <t>Frog</t>
   </si>
   <si>
-    <t>MushRoom</t>
+    <t>PurpleBeatle</t>
   </si>
   <si>
     <t>Kabu</t>
-  </si>
-  <si>
-    <t>PurpleBeatle</t>
   </si>
   <si>
     <t>NormalBear</t>
@@ -662,7 +662,7 @@
         <v>100</v>
       </c>
       <c r="D9" s="5">
-        <v>150</v>
+        <v>80</v>
       </c>
       <c r="E9" s="5">
         <v>500</v>
@@ -697,7 +697,7 @@
         <v>100</v>
       </c>
       <c r="D10" s="5">
-        <v>150</v>
+        <v>80</v>
       </c>
       <c r="E10" s="5">
         <v>500</v>
@@ -732,7 +732,7 @@
         <v>100</v>
       </c>
       <c r="D11" s="5">
-        <v>150</v>
+        <v>80</v>
       </c>
       <c r="E11" s="5">
         <v>500</v>
@@ -767,7 +767,7 @@
         <v>100</v>
       </c>
       <c r="D12" s="5">
-        <v>150</v>
+        <v>80</v>
       </c>
       <c r="E12" s="5">
         <v>500</v>
@@ -802,7 +802,7 @@
         <v>100</v>
       </c>
       <c r="D13" s="5">
-        <v>150</v>
+        <v>80</v>
       </c>
       <c r="E13" s="5">
         <v>500</v>
@@ -837,7 +837,7 @@
         <v>100</v>
       </c>
       <c r="D14" s="5">
-        <v>150</v>
+        <v>80</v>
       </c>
       <c r="E14" s="5">
         <v>500</v>
@@ -846,13 +846,13 @@
         <v>100</v>
       </c>
       <c r="G14" s="5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H14" s="5">
         <v>50</v>
       </c>
       <c r="I14" s="5">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="J14" s="5">
         <v>0</v>
@@ -872,7 +872,7 @@
         <v>100</v>
       </c>
       <c r="D15" s="5">
-        <v>150</v>
+        <v>80</v>
       </c>
       <c r="E15" s="5">
         <v>500</v>
@@ -881,13 +881,13 @@
         <v>100</v>
       </c>
       <c r="G15" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H15" s="5">
         <v>50</v>
       </c>
       <c r="I15" s="5">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="J15" s="5">
         <v>0</v>
@@ -907,7 +907,7 @@
         <v>200</v>
       </c>
       <c r="D16" s="5">
-        <v>150</v>
+        <v>80</v>
       </c>
       <c r="E16" s="5">
         <v>500</v>

</xml_diff>

<commit_message>
[Feat] (Client) Stop Boss Monster When It Dies & Extend World Resolution After PaperBurn Of Boss Monster
</commit_message>
<xml_diff>
--- a/CharacterStats.xlsx
+++ b/CharacterStats.xlsx
@@ -72,22 +72,22 @@
     <t>Normal</t>
   </si>
   <si>
+    <t>Chicken</t>
+  </si>
+  <si>
     <t>YellowBird</t>
   </si>
   <si>
-    <t>Chicken</t>
+    <t>Frog</t>
   </si>
   <si>
     <t>MushRoom</t>
   </si>
   <si>
-    <t>Frog</t>
+    <t>Kabu</t>
   </si>
   <si>
     <t>PurpleBeatle</t>
-  </si>
-  <si>
-    <t>Kabu</t>
   </si>
   <si>
     <t>NormalBear</t>
@@ -846,13 +846,13 @@
         <v>100</v>
       </c>
       <c r="G14" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H14" s="5">
         <v>50</v>
       </c>
       <c r="I14" s="5">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="J14" s="5">
         <v>0</v>
@@ -881,13 +881,13 @@
         <v>100</v>
       </c>
       <c r="G15" s="5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H15" s="5">
         <v>50</v>
       </c>
       <c r="I15" s="5">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="J15" s="5">
         <v>0</v>
@@ -1248,7 +1248,7 @@
         <v>0</v>
       </c>
       <c r="H25" s="5">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="I25" s="5">
         <v>250</v>

</xml_diff>

<commit_message>
[Feat] (Client) Register "UltimateAttack" Key To Player2D
</commit_message>
<xml_diff>
--- a/CharacterStats.xlsx
+++ b/CharacterStats.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="60" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="61" uniqueCount="41">
   <si>
     <t>Created by LibXL trial version 4.0.3. Please buy the LibXL full version for removing this message.</t>
   </si>
@@ -72,24 +72,24 @@
     <t>Normal</t>
   </si>
   <si>
+    <t>YellowBird</t>
+  </si>
+  <si>
     <t>Chicken</t>
   </si>
   <si>
-    <t>YellowBird</t>
+    <t>MushRoom</t>
   </si>
   <si>
     <t>Frog</t>
   </si>
   <si>
-    <t>MushRoom</t>
+    <t>PurpleBeatle</t>
   </si>
   <si>
     <t>Kabu</t>
   </si>
   <si>
-    <t>PurpleBeatle</t>
-  </si>
-  <si>
     <t>NormalBear</t>
   </si>
   <si>
@@ -130,6 +130,9 @@
   </si>
   <si>
     <t>BossHammer</t>
+  </si>
+  <si>
+    <t>Buy me !</t>
   </si>
   <si>
     <t>BossScissor</t>
@@ -846,13 +849,13 @@
         <v>100</v>
       </c>
       <c r="G14" s="5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H14" s="5">
         <v>50</v>
       </c>
       <c r="I14" s="5">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="J14" s="5">
         <v>0</v>
@@ -881,13 +884,13 @@
         <v>100</v>
       </c>
       <c r="G15" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H15" s="5">
         <v>50</v>
       </c>
       <c r="I15" s="5">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="J15" s="5">
         <v>0</v>
@@ -1286,8 +1289,8 @@
       <c r="G26" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="H26" s="5">
-        <v>100</v>
+      <c r="H26" s="5" t="s">
+        <v>39</v>
       </c>
       <c r="I26" s="5">
         <v>200</v>
@@ -1305,7 +1308,7 @@
     </row>
     <row r="27" ht="28" customHeight="true" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B27" s="5" t="s">
         <v>36</v>

</xml_diff>

<commit_message>
[Feat] (Client) Create CUltimateAttackWidget Widget Which Appear Specially When Player Ultimate Attack
</commit_message>
<xml_diff>
--- a/CharacterStats.xlsx
+++ b/CharacterStats.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="61" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="60" uniqueCount="40">
   <si>
     <t>Created by LibXL trial version 4.0.3. Please buy the LibXL full version for removing this message.</t>
   </si>
@@ -130,9 +130,6 @@
   </si>
   <si>
     <t>BossHammer</t>
-  </si>
-  <si>
-    <t>Buy me !</t>
   </si>
   <si>
     <t>BossScissor</t>
@@ -1289,8 +1286,8 @@
       <c r="G26" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="H26" s="5" t="s">
-        <v>39</v>
+      <c r="H26" s="5">
+        <v>0</v>
       </c>
       <c r="I26" s="5">
         <v>200</v>
@@ -1308,7 +1305,7 @@
     </row>
     <row r="27" ht="28" customHeight="true" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B27" s="5" t="s">
         <v>36</v>

</xml_diff>

<commit_message>
[Feat] (Client) CUltimateAttackWidget Created When Player Ultimate Attack  & Slide From Right To Left
</commit_message>
<xml_diff>
--- a/CharacterStats.xlsx
+++ b/CharacterStats.xlsx
@@ -1157,7 +1157,7 @@
         <v>30</v>
       </c>
       <c r="C23" s="5">
-        <v>300</v>
+        <v>0</v>
       </c>
       <c r="D23" s="5">
         <v>550</v>
@@ -1175,7 +1175,7 @@
         <v>150</v>
       </c>
       <c r="I23" s="5">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="J23" s="5">
         <v>50</v>

</xml_diff>

<commit_message>
[Feat] (Client) Create CBeamUltimate Class Which Is An Ultimate AttackEffect Made By BeamKirby
</commit_message>
<xml_diff>
--- a/CharacterStats.xlsx
+++ b/CharacterStats.xlsx
@@ -72,22 +72,22 @@
     <t>Normal</t>
   </si>
   <si>
+    <t>Chicken</t>
+  </si>
+  <si>
     <t>YellowBird</t>
   </si>
   <si>
-    <t>Chicken</t>
+    <t>Frog</t>
   </si>
   <si>
     <t>MushRoom</t>
   </si>
   <si>
-    <t>Frog</t>
+    <t>Kabu</t>
   </si>
   <si>
     <t>PurpleBeatle</t>
-  </si>
-  <si>
-    <t>Kabu</t>
   </si>
   <si>
     <t>NormalBear</t>
@@ -846,13 +846,13 @@
         <v>100</v>
       </c>
       <c r="G14" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H14" s="5">
         <v>50</v>
       </c>
       <c r="I14" s="5">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="J14" s="5">
         <v>0</v>
@@ -881,13 +881,13 @@
         <v>100</v>
       </c>
       <c r="G15" s="5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H15" s="5">
         <v>50</v>
       </c>
       <c r="I15" s="5">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="J15" s="5">
         <v>0</v>
@@ -1135,7 +1135,7 @@
         <v>1</v>
       </c>
       <c r="H22" s="5">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="I22" s="5">
         <v>100</v>
@@ -1163,7 +1163,7 @@
         <v>550</v>
       </c>
       <c r="E23" s="5">
-        <v>800</v>
+        <v>0</v>
       </c>
       <c r="F23" s="5">
         <v>100</v>
@@ -1233,7 +1233,7 @@
         <v>36</v>
       </c>
       <c r="C25" s="5">
-        <v>5000</v>
+        <v>0</v>
       </c>
       <c r="D25" s="5">
         <v>1100</v>
@@ -1281,7 +1281,7 @@
         <v>1000</v>
       </c>
       <c r="F26" s="5">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="G26" s="5" t="b">
         <v>1</v>

</xml_diff>

<commit_message>
[Feat] (Client) Create UlmateAttack, UndoUltimateAttack Function In Player2D , Which Is Activated At The Start, End Of Player Ultimate Attack
</commit_message>
<xml_diff>
--- a/CharacterStats.xlsx
+++ b/CharacterStats.xlsx
@@ -72,22 +72,22 @@
     <t>Normal</t>
   </si>
   <si>
+    <t>YellowBird</t>
+  </si>
+  <si>
     <t>Chicken</t>
   </si>
   <si>
-    <t>YellowBird</t>
+    <t>MushRoom</t>
   </si>
   <si>
     <t>Frog</t>
   </si>
   <si>
-    <t>MushRoom</t>
+    <t>PurpleBeatle</t>
   </si>
   <si>
     <t>Kabu</t>
-  </si>
-  <si>
-    <t>PurpleBeatle</t>
   </si>
   <si>
     <t>NormalBear</t>
@@ -846,13 +846,13 @@
         <v>100</v>
       </c>
       <c r="G14" s="5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H14" s="5">
         <v>50</v>
       </c>
       <c r="I14" s="5">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="J14" s="5">
         <v>0</v>
@@ -881,13 +881,13 @@
         <v>100</v>
       </c>
       <c r="G15" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H15" s="5">
         <v>50</v>
       </c>
       <c r="I15" s="5">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="J15" s="5">
         <v>0</v>

</xml_diff>

<commit_message>
[Feat] (Client) Apply Different Alpha BackGround Image According To Different Kirby Special State
</commit_message>
<xml_diff>
--- a/CharacterStats.xlsx
+++ b/CharacterStats.xlsx
@@ -72,22 +72,22 @@
     <t>Normal</t>
   </si>
   <si>
+    <t>Chicken</t>
+  </si>
+  <si>
     <t>YellowBird</t>
   </si>
   <si>
-    <t>Chicken</t>
+    <t>Frog</t>
   </si>
   <si>
     <t>MushRoom</t>
   </si>
   <si>
-    <t>Frog</t>
+    <t>Kabu</t>
   </si>
   <si>
     <t>PurpleBeatle</t>
-  </si>
-  <si>
-    <t>Kabu</t>
   </si>
   <si>
     <t>NormalBear</t>
@@ -846,13 +846,13 @@
         <v>100</v>
       </c>
       <c r="G14" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H14" s="5">
         <v>50</v>
       </c>
       <c r="I14" s="5">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="J14" s="5">
         <v>0</v>
@@ -881,13 +881,13 @@
         <v>100</v>
       </c>
       <c r="G15" s="5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H15" s="5">
         <v>50</v>
       </c>
       <c r="I15" s="5">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="J15" s="5">
         <v>0</v>
@@ -1141,7 +1141,7 @@
         <v>100</v>
       </c>
       <c r="J22" s="5">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="K22" s="5"/>
       <c r="L22" s="5"/>

</xml_diff>

<commit_message>
[Feat] (Client) BombKirby Bomb Throw Angle Randomly Set
</commit_message>
<xml_diff>
--- a/CharacterStats.xlsx
+++ b/CharacterStats.xlsx
@@ -72,22 +72,22 @@
     <t>Normal</t>
   </si>
   <si>
+    <t>YellowBird</t>
+  </si>
+  <si>
     <t>Chicken</t>
   </si>
   <si>
-    <t>YellowBird</t>
+    <t>MushRoom</t>
   </si>
   <si>
     <t>Frog</t>
   </si>
   <si>
-    <t>MushRoom</t>
+    <t>PurpleBeatle</t>
   </si>
   <si>
     <t>Kabu</t>
-  </si>
-  <si>
-    <t>PurpleBeatle</t>
   </si>
   <si>
     <t>NormalBear</t>
@@ -846,13 +846,13 @@
         <v>100</v>
       </c>
       <c r="G14" s="5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H14" s="5">
         <v>50</v>
       </c>
       <c r="I14" s="5">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="J14" s="5">
         <v>0</v>
@@ -881,13 +881,13 @@
         <v>100</v>
       </c>
       <c r="G15" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H15" s="5">
         <v>50</v>
       </c>
       <c r="I15" s="5">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="J15" s="5">
         <v>0</v>

</xml_diff>

<commit_message>
[Feat] (Client) Apply Ultimate Attack Logic To Sword Kirby
</commit_message>
<xml_diff>
--- a/CharacterStats.xlsx
+++ b/CharacterStats.xlsx
@@ -72,22 +72,22 @@
     <t>Normal</t>
   </si>
   <si>
+    <t>Chicken</t>
+  </si>
+  <si>
     <t>YellowBird</t>
   </si>
   <si>
-    <t>Chicken</t>
+    <t>Frog</t>
   </si>
   <si>
     <t>MushRoom</t>
   </si>
   <si>
-    <t>Frog</t>
+    <t>Kabu</t>
   </si>
   <si>
     <t>PurpleBeatle</t>
-  </si>
-  <si>
-    <t>Kabu</t>
   </si>
   <si>
     <t>NormalBear</t>
@@ -846,13 +846,13 @@
         <v>100</v>
       </c>
       <c r="G14" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H14" s="5">
         <v>50</v>
       </c>
       <c r="I14" s="5">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="J14" s="5">
         <v>0</v>
@@ -881,13 +881,13 @@
         <v>100</v>
       </c>
       <c r="G15" s="5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H15" s="5">
         <v>50</v>
       </c>
       <c r="I15" s="5">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="J15" s="5">
         <v>0</v>
@@ -1135,7 +1135,7 @@
         <v>1</v>
       </c>
       <c r="H22" s="5">
-        <v>0</v>
+        <v>150</v>
       </c>
       <c r="I22" s="5">
         <v>100</v>
@@ -1157,13 +1157,13 @@
         <v>30</v>
       </c>
       <c r="C23" s="5">
-        <v>0</v>
+        <v>300</v>
       </c>
       <c r="D23" s="5">
         <v>550</v>
       </c>
       <c r="E23" s="5">
-        <v>0</v>
+        <v>700</v>
       </c>
       <c r="F23" s="5">
         <v>100</v>
@@ -1233,10 +1233,10 @@
         <v>36</v>
       </c>
       <c r="C25" s="5">
-        <v>0</v>
+        <v>5000</v>
       </c>
       <c r="D25" s="5">
-        <v>1100</v>
+        <v>900</v>
       </c>
       <c r="E25" s="5">
         <v>1000</v>
@@ -1248,7 +1248,7 @@
         <v>0</v>
       </c>
       <c r="H25" s="5">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="I25" s="5">
         <v>250</v>
@@ -1260,7 +1260,7 @@
         <v>550</v>
       </c>
       <c r="L25" s="5">
-        <v>1100</v>
+        <v>0</v>
       </c>
       <c r="M25" s="5"/>
     </row>
@@ -1281,13 +1281,13 @@
         <v>1000</v>
       </c>
       <c r="F26" s="5">
-        <v>0</v>
+        <v>150</v>
       </c>
       <c r="G26" s="5" t="b">
         <v>1</v>
       </c>
       <c r="H26" s="5">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="I26" s="5">
         <v>200</v>

</xml_diff>

<commit_message>
[Feat] (Client) Apply Ultimate Attack Logic To Fight Kirby
</commit_message>
<xml_diff>
--- a/CharacterStats.xlsx
+++ b/CharacterStats.xlsx
@@ -72,22 +72,22 @@
     <t>Normal</t>
   </si>
   <si>
+    <t>YellowBird</t>
+  </si>
+  <si>
     <t>Chicken</t>
   </si>
   <si>
-    <t>YellowBird</t>
+    <t>MushRoom</t>
   </si>
   <si>
     <t>Frog</t>
   </si>
   <si>
-    <t>MushRoom</t>
+    <t>PurpleBeatle</t>
   </si>
   <si>
     <t>Kabu</t>
-  </si>
-  <si>
-    <t>PurpleBeatle</t>
   </si>
   <si>
     <t>NormalBear</t>
@@ -846,13 +846,13 @@
         <v>100</v>
       </c>
       <c r="G14" s="5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H14" s="5">
         <v>50</v>
       </c>
       <c r="I14" s="5">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="J14" s="5">
         <v>0</v>
@@ -881,13 +881,13 @@
         <v>100</v>
       </c>
       <c r="G15" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H15" s="5">
         <v>50</v>
       </c>
       <c r="I15" s="5">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="J15" s="5">
         <v>0</v>

</xml_diff>

<commit_message>
[Feat] (Client) Create RandomStar When Monster Or Block Destroyed
</commit_message>
<xml_diff>
--- a/CharacterStats.xlsx
+++ b/CharacterStats.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="60" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="61" uniqueCount="41">
   <si>
     <t>Created by LibXL trial version 4.0.3. Please buy the LibXL full version for removing this message.</t>
   </si>
@@ -72,24 +72,24 @@
     <t>Normal</t>
   </si>
   <si>
+    <t>Chicken</t>
+  </si>
+  <si>
     <t>YellowBird</t>
   </si>
   <si>
-    <t>Chicken</t>
+    <t>Frog</t>
   </si>
   <si>
     <t>MushRoom</t>
   </si>
   <si>
-    <t>Frog</t>
+    <t>Kabu</t>
   </si>
   <si>
     <t>PurpleBeatle</t>
   </si>
   <si>
-    <t>Kabu</t>
-  </si>
-  <si>
     <t>NormalBear</t>
   </si>
   <si>
@@ -118,6 +118,9 @@
   </si>
   <si>
     <t>Sword</t>
+  </si>
+  <si>
+    <t>Buy me !</t>
   </si>
   <si>
     <t>BossPenguin</t>
@@ -846,13 +849,13 @@
         <v>100</v>
       </c>
       <c r="G14" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H14" s="5">
         <v>50</v>
       </c>
       <c r="I14" s="5">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="J14" s="5">
         <v>0</v>
@@ -881,13 +884,13 @@
         <v>100</v>
       </c>
       <c r="G15" s="5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H15" s="5">
         <v>50</v>
       </c>
       <c r="I15" s="5">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="J15" s="5">
         <v>0</v>
@@ -1174,8 +1177,8 @@
       <c r="H23" s="5">
         <v>150</v>
       </c>
-      <c r="I23" s="5">
-        <v>0</v>
+      <c r="I23" s="5" t="s">
+        <v>35</v>
       </c>
       <c r="J23" s="5">
         <v>50</v>
@@ -1188,10 +1191,10 @@
     </row>
     <row r="24" ht="28" customHeight="true" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C24" s="5">
         <v>5000</v>
@@ -1227,10 +1230,10 @@
     </row>
     <row r="25" ht="28" customHeight="true" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B25" s="5" t="s">
         <v>37</v>
-      </c>
-      <c r="B25" s="5" t="s">
-        <v>36</v>
       </c>
       <c r="C25" s="5">
         <v>5000</v>
@@ -1266,10 +1269,10 @@
     </row>
     <row r="26" ht="28" customHeight="true" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C26" s="5">
         <v>3000</v>
@@ -1305,10 +1308,10 @@
     </row>
     <row r="27" ht="28" customHeight="true" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C27" s="5">
         <v>3000</v>

</xml_diff>

<commit_message>
[Feat] (Client) Call Collision Callback Of Monster Attack Only When It Collider With Player Body Collider
</commit_message>
<xml_diff>
--- a/CharacterStats.xlsx
+++ b/CharacterStats.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="61" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="60" uniqueCount="40">
   <si>
     <t>Created by LibXL trial version 4.0.3. Please buy the LibXL full version for removing this message.</t>
   </si>
@@ -118,9 +118,6 @@
   </si>
   <si>
     <t>Sword</t>
-  </si>
-  <si>
-    <t>Buy me !</t>
   </si>
   <si>
     <t>BossPenguin</t>
@@ -1027,7 +1024,7 @@
         <v>1</v>
       </c>
       <c r="H19" s="5">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="I19" s="5">
         <v>100</v>
@@ -1064,7 +1061,7 @@
         <v>1</v>
       </c>
       <c r="H20" s="5">
-        <v>150</v>
+        <v>90</v>
       </c>
       <c r="I20" s="5">
         <v>100</v>
@@ -1101,7 +1098,7 @@
         <v>1</v>
       </c>
       <c r="H21" s="5">
-        <v>150</v>
+        <v>90</v>
       </c>
       <c r="I21" s="5">
         <v>100</v>
@@ -1138,7 +1135,7 @@
         <v>1</v>
       </c>
       <c r="H22" s="5">
-        <v>150</v>
+        <v>90</v>
       </c>
       <c r="I22" s="5">
         <v>100</v>
@@ -1175,10 +1172,10 @@
         <v>1</v>
       </c>
       <c r="H23" s="5">
-        <v>150</v>
-      </c>
-      <c r="I23" s="5" t="s">
-        <v>35</v>
+        <v>90</v>
+      </c>
+      <c r="I23" s="5">
+        <v>0</v>
       </c>
       <c r="J23" s="5">
         <v>50</v>
@@ -1191,10 +1188,10 @@
     </row>
     <row r="24" ht="28" customHeight="true" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B24" s="5" t="s">
         <v>36</v>
-      </c>
-      <c r="B24" s="5" t="s">
-        <v>37</v>
       </c>
       <c r="C24" s="5">
         <v>5000</v>
@@ -1212,7 +1209,7 @@
         <v>1</v>
       </c>
       <c r="H24" s="5">
-        <v>150</v>
+        <v>90</v>
       </c>
       <c r="I24" s="5">
         <v>300</v>
@@ -1230,10 +1227,10 @@
     </row>
     <row r="25" ht="28" customHeight="true" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C25" s="5">
         <v>5000</v>
@@ -1251,7 +1248,7 @@
         <v>0</v>
       </c>
       <c r="H25" s="5">
-        <v>50</v>
+        <v>90</v>
       </c>
       <c r="I25" s="5">
         <v>250</v>
@@ -1269,10 +1266,10 @@
     </row>
     <row r="26" ht="28" customHeight="true" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C26" s="5">
         <v>3000</v>
@@ -1290,7 +1287,7 @@
         <v>1</v>
       </c>
       <c r="H26" s="5">
-        <v>50</v>
+        <v>90</v>
       </c>
       <c r="I26" s="5">
         <v>200</v>
@@ -1308,10 +1305,10 @@
     </row>
     <row r="27" ht="28" customHeight="true" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C27" s="5">
         <v>3000</v>
@@ -1329,7 +1326,7 @@
         <v>1</v>
       </c>
       <c r="H27" s="5">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="I27" s="5">
         <v>250</v>

</xml_diff>

<commit_message>
[Feat] (Client) Make PlayerClone Class & Make Cloned Kirby With Opacity Continuosly Decreasing When Player Slide Attack Or Dash
</commit_message>
<xml_diff>
--- a/CharacterStats.xlsx
+++ b/CharacterStats.xlsx
@@ -72,22 +72,22 @@
     <t>Normal</t>
   </si>
   <si>
+    <t>YellowBird</t>
+  </si>
+  <si>
     <t>Chicken</t>
   </si>
   <si>
-    <t>YellowBird</t>
+    <t>MushRoom</t>
   </si>
   <si>
     <t>Frog</t>
   </si>
   <si>
-    <t>MushRoom</t>
+    <t>PurpleBeatle</t>
   </si>
   <si>
     <t>Kabu</t>
-  </si>
-  <si>
-    <t>PurpleBeatle</t>
   </si>
   <si>
     <t>NormalBear</t>
@@ -846,13 +846,13 @@
         <v>100</v>
       </c>
       <c r="G14" s="5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H14" s="5">
         <v>50</v>
       </c>
       <c r="I14" s="5">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="J14" s="5">
         <v>0</v>
@@ -881,13 +881,13 @@
         <v>100</v>
       </c>
       <c r="G15" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H15" s="5">
         <v>50</v>
       </c>
       <c r="I15" s="5">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="J15" s="5">
         <v>0</v>

</xml_diff>

<commit_message>
[Feat] (Client) Make Player Clone Effect When Special Kirby State Special Attack
</commit_message>
<xml_diff>
--- a/CharacterStats.xlsx
+++ b/CharacterStats.xlsx
@@ -72,22 +72,22 @@
     <t>Normal</t>
   </si>
   <si>
+    <t>Chicken</t>
+  </si>
+  <si>
     <t>YellowBird</t>
   </si>
   <si>
-    <t>Chicken</t>
+    <t>Frog</t>
   </si>
   <si>
     <t>MushRoom</t>
   </si>
   <si>
-    <t>Frog</t>
+    <t>Kabu</t>
   </si>
   <si>
     <t>PurpleBeatle</t>
-  </si>
-  <si>
-    <t>Kabu</t>
   </si>
   <si>
     <t>NormalBear</t>
@@ -846,13 +846,13 @@
         <v>100</v>
       </c>
       <c r="G14" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H14" s="5">
         <v>50</v>
       </c>
       <c r="I14" s="5">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="J14" s="5">
         <v>0</v>
@@ -881,13 +881,13 @@
         <v>100</v>
       </c>
       <c r="G15" s="5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H15" s="5">
         <v>50</v>
       </c>
       <c r="I15" s="5">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="J15" s="5">
         <v>0</v>

</xml_diff>

<commit_message>
[Feat] (Client) Pullright, LeftCollider Of Player Increase its Size When Player Pull
</commit_message>
<xml_diff>
--- a/CharacterStats.xlsx
+++ b/CharacterStats.xlsx
@@ -72,22 +72,22 @@
     <t>Normal</t>
   </si>
   <si>
+    <t>YellowBird</t>
+  </si>
+  <si>
     <t>Chicken</t>
   </si>
   <si>
-    <t>YellowBird</t>
+    <t>MushRoom</t>
   </si>
   <si>
     <t>Frog</t>
   </si>
   <si>
-    <t>MushRoom</t>
+    <t>PurpleBeatle</t>
   </si>
   <si>
     <t>Kabu</t>
-  </si>
-  <si>
-    <t>PurpleBeatle</t>
   </si>
   <si>
     <t>NormalBear</t>
@@ -846,13 +846,13 @@
         <v>100</v>
       </c>
       <c r="G14" s="5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H14" s="5">
         <v>50</v>
       </c>
       <c r="I14" s="5">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="J14" s="5">
         <v>0</v>
@@ -881,13 +881,13 @@
         <v>100</v>
       </c>
       <c r="G15" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H15" s="5">
         <v>50</v>
       </c>
       <c r="I15" s="5">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="J15" s="5">
         <v>0</v>

</xml_diff>

<commit_message>
[Fix] (Client) Player , Camera Pos Limited Inside Boss World Resolution
</commit_message>
<xml_diff>
--- a/CharacterStats.xlsx
+++ b/CharacterStats.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="60" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="61" uniqueCount="41">
   <si>
     <t>Created by LibXL trial version 4.0.3. Please buy the LibXL full version for removing this message.</t>
   </si>
@@ -127,6 +127,9 @@
   </si>
   <si>
     <t>BossTree</t>
+  </si>
+  <si>
+    <t>Buy me !</t>
   </si>
   <si>
     <t>BossHammer</t>
@@ -1232,8 +1235,8 @@
       <c r="B25" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="C25" s="5">
-        <v>5000</v>
+      <c r="C25" s="5" t="s">
+        <v>38</v>
       </c>
       <c r="D25" s="5">
         <v>900</v>
@@ -1266,7 +1269,7 @@
     </row>
     <row r="26" ht="28" customHeight="true" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B26" s="5" t="s">
         <v>36</v>
@@ -1305,7 +1308,7 @@
     </row>
     <row r="27" ht="28" customHeight="true" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B27" s="5" t="s">
         <v>36</v>

</xml_diff>

<commit_message>
[Feat] (Client) Create CScary Class Which Represent Scary Monster
</commit_message>
<xml_diff>
--- a/CharacterStats.xlsx
+++ b/CharacterStats.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="61" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="60" uniqueCount="40">
   <si>
     <t>Created by LibXL trial version 4.0.3. Please buy the LibXL full version for removing this message.</t>
   </si>
@@ -72,24 +72,24 @@
     <t>Normal</t>
   </si>
   <si>
+    <t>Chicken</t>
+  </si>
+  <si>
     <t>YellowBird</t>
   </si>
   <si>
-    <t>Chicken</t>
+    <t>Frog</t>
   </si>
   <si>
     <t>MushRoom</t>
   </si>
   <si>
-    <t>Frog</t>
+    <t>Kabu</t>
   </si>
   <si>
     <t>PurpleBeatle</t>
   </si>
   <si>
-    <t>Kabu</t>
-  </si>
-  <si>
     <t>NormalBear</t>
   </si>
   <si>
@@ -127,9 +127,6 @@
   </si>
   <si>
     <t>BossTree</t>
-  </si>
-  <si>
-    <t>Buy me !</t>
   </si>
   <si>
     <t>BossHammer</t>
@@ -849,13 +846,13 @@
         <v>100</v>
       </c>
       <c r="G14" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H14" s="5">
         <v>50</v>
       </c>
       <c r="I14" s="5">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="J14" s="5">
         <v>0</v>
@@ -884,13 +881,13 @@
         <v>100</v>
       </c>
       <c r="G15" s="5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H15" s="5">
         <v>50</v>
       </c>
       <c r="I15" s="5">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="J15" s="5">
         <v>0</v>
@@ -1235,8 +1232,8 @@
       <c r="B25" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="C25" s="5" t="s">
-        <v>38</v>
+      <c r="C25" s="5">
+        <v>0</v>
       </c>
       <c r="D25" s="5">
         <v>900</v>
@@ -1269,7 +1266,7 @@
     </row>
     <row r="26" ht="28" customHeight="true" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B26" s="5" t="s">
         <v>36</v>
@@ -1308,7 +1305,7 @@
     </row>
     <row r="27" ht="28" customHeight="true" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B27" s="5" t="s">
         <v>36</v>

</xml_diff>

<commit_message>
[Feat] (Client) Hide Line Behind TileMap
</commit_message>
<xml_diff>
--- a/CharacterStats.xlsx
+++ b/CharacterStats.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="60" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="64" uniqueCount="42">
   <si>
     <t>Created by LibXL trial version 4.0.3. Please buy the LibXL full version for removing this message.</t>
   </si>
@@ -72,27 +72,36 @@
     <t>Normal</t>
   </si>
   <si>
+    <t>YellowBird</t>
+  </si>
+  <si>
     <t>Chicken</t>
   </si>
   <si>
-    <t>YellowBird</t>
+    <t>MushRoom</t>
   </si>
   <si>
     <t>Frog</t>
   </si>
   <si>
-    <t>MushRoom</t>
+    <t>PurpleBeatle</t>
   </si>
   <si>
     <t>Kabu</t>
   </si>
   <si>
-    <t>PurpleBeatle</t>
+    <t>BossDyna</t>
+  </si>
+  <si>
+    <t>Boss</t>
   </si>
   <si>
     <t>NormalBear</t>
   </si>
   <si>
+    <t>Scary</t>
+  </si>
+  <si>
     <t>Squid</t>
   </si>
   <si>
@@ -121,9 +130,6 @@
   </si>
   <si>
     <t>BossPenguin</t>
-  </si>
-  <si>
-    <t>Boss</t>
   </si>
   <si>
     <t>BossTree</t>
@@ -846,13 +852,13 @@
         <v>100</v>
       </c>
       <c r="G14" s="5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H14" s="5">
         <v>50</v>
       </c>
       <c r="I14" s="5">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="J14" s="5">
         <v>0</v>
@@ -881,13 +887,13 @@
         <v>100</v>
       </c>
       <c r="G15" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H15" s="5">
         <v>50</v>
       </c>
       <c r="I15" s="5">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="J15" s="5">
         <v>0</v>
@@ -901,63 +907,67 @@
         <v>25</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="C16" s="5">
-        <v>200</v>
+        <v>5000</v>
       </c>
       <c r="D16" s="5">
-        <v>80</v>
+        <v>1005</v>
       </c>
       <c r="E16" s="5">
-        <v>500</v>
+        <v>1400</v>
       </c>
       <c r="F16" s="5">
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="G16" s="5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H16" s="5">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="I16" s="5">
-        <v>160</v>
+        <v>350</v>
       </c>
       <c r="J16" s="5">
         <v>0</v>
       </c>
-      <c r="K16" s="5"/>
-      <c r="L16" s="5"/>
+      <c r="K16" s="5">
+        <v>600</v>
+      </c>
+      <c r="L16" s="5">
+        <v>1000</v>
+      </c>
       <c r="M16" s="5"/>
     </row>
     <row r="17" ht="28" customHeight="true" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="C17" s="5">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="D17" s="5">
-        <v>65</v>
+        <v>40</v>
       </c>
       <c r="E17" s="5">
-        <v>550</v>
+        <v>500</v>
       </c>
       <c r="F17" s="5">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="G17" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H17" s="5">
-        <v>50</v>
+        <v>80</v>
       </c>
       <c r="I17" s="5">
-        <v>100</v>
+        <v>160</v>
       </c>
       <c r="J17" s="5">
         <v>0</v>
@@ -971,28 +981,28 @@
         <v>28</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="C18" s="5">
         <v>100</v>
       </c>
       <c r="D18" s="5">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="E18" s="5">
-        <v>550</v>
+        <v>400</v>
       </c>
       <c r="F18" s="5">
         <v>100</v>
       </c>
       <c r="G18" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H18" s="5">
         <v>50</v>
       </c>
       <c r="I18" s="5">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="J18" s="5">
         <v>0</v>
@@ -1009,22 +1019,22 @@
         <v>30</v>
       </c>
       <c r="C19" s="5">
-        <v>300</v>
+        <v>100</v>
       </c>
       <c r="D19" s="5">
-        <v>450</v>
+        <v>60</v>
       </c>
       <c r="E19" s="5">
-        <v>600</v>
+        <v>200</v>
       </c>
       <c r="F19" s="5">
         <v>100</v>
       </c>
       <c r="G19" s="5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H19" s="5">
-        <v>90</v>
+        <v>50</v>
       </c>
       <c r="I19" s="5">
         <v>100</v>
@@ -1034,9 +1044,7 @@
       </c>
       <c r="K19" s="5"/>
       <c r="L19" s="5"/>
-      <c r="M19" s="5" t="s">
-        <v>29</v>
-      </c>
+      <c r="M19" s="5"/>
     </row>
     <row r="20" ht="28" customHeight="true" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
@@ -1046,22 +1054,22 @@
         <v>30</v>
       </c>
       <c r="C20" s="5">
-        <v>300</v>
+        <v>100</v>
       </c>
       <c r="D20" s="5">
-        <v>450</v>
+        <v>60</v>
       </c>
       <c r="E20" s="5">
-        <v>550</v>
+        <v>200</v>
       </c>
       <c r="F20" s="5">
         <v>100</v>
       </c>
       <c r="G20" s="5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H20" s="5">
-        <v>90</v>
+        <v>50</v>
       </c>
       <c r="I20" s="5">
         <v>100</v>
@@ -1071,22 +1079,20 @@
       </c>
       <c r="K20" s="5"/>
       <c r="L20" s="5"/>
-      <c r="M20" s="5" t="s">
-        <v>31</v>
-      </c>
+      <c r="M20" s="5"/>
     </row>
     <row r="21" ht="28" customHeight="true" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>32</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C21" s="5">
         <v>300</v>
       </c>
       <c r="D21" s="5">
-        <v>350</v>
+        <v>450</v>
       </c>
       <c r="E21" s="5">
         <v>600</v>
@@ -1114,10 +1120,10 @@
     </row>
     <row r="22" ht="28" customHeight="true" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B22" s="5" t="s">
         <v>33</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>30</v>
       </c>
       <c r="C22" s="5">
         <v>300</v>
@@ -1126,7 +1132,7 @@
         <v>450</v>
       </c>
       <c r="E22" s="5">
-        <v>800</v>
+        <v>550</v>
       </c>
       <c r="F22" s="5">
         <v>100</v>
@@ -1146,24 +1152,24 @@
       <c r="K22" s="5"/>
       <c r="L22" s="5"/>
       <c r="M22" s="5" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="23" ht="28" customHeight="true" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C23" s="5">
         <v>300</v>
       </c>
       <c r="D23" s="5">
-        <v>550</v>
+        <v>350</v>
       </c>
       <c r="E23" s="5">
-        <v>700</v>
+        <v>600</v>
       </c>
       <c r="F23" s="5">
         <v>100</v>
@@ -1175,35 +1181,35 @@
         <v>90</v>
       </c>
       <c r="I23" s="5">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="J23" s="5">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="K23" s="5"/>
       <c r="L23" s="5"/>
       <c r="M23" s="5" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="24" ht="28" customHeight="true" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C24" s="5">
-        <v>5000</v>
+        <v>300</v>
       </c>
       <c r="D24" s="5">
-        <v>600</v>
+        <v>450</v>
       </c>
       <c r="E24" s="5">
-        <v>1200</v>
+        <v>800</v>
       </c>
       <c r="F24" s="5">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="G24" s="5" t="b">
         <v>1</v>
@@ -1212,76 +1218,72 @@
         <v>90</v>
       </c>
       <c r="I24" s="5">
-        <v>300</v>
+        <v>100</v>
       </c>
       <c r="J24" s="5">
-        <v>60</v>
-      </c>
-      <c r="K24" s="5">
-        <v>400</v>
-      </c>
-      <c r="L24" s="5">
-        <v>600</v>
-      </c>
-      <c r="M24" s="5"/>
+        <v>50</v>
+      </c>
+      <c r="K24" s="5"/>
+      <c r="L24" s="5"/>
+      <c r="M24" s="5" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="25" ht="28" customHeight="true" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
         <v>37</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C25" s="5">
-        <v>0</v>
+        <v>300</v>
       </c>
       <c r="D25" s="5">
-        <v>900</v>
+        <v>550</v>
       </c>
       <c r="E25" s="5">
-        <v>1000</v>
+        <v>800</v>
       </c>
       <c r="F25" s="5">
         <v>100</v>
       </c>
       <c r="G25" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H25" s="5">
         <v>90</v>
       </c>
       <c r="I25" s="5">
-        <v>250</v>
+        <v>100</v>
       </c>
       <c r="J25" s="5">
-        <v>0</v>
-      </c>
-      <c r="K25" s="5">
-        <v>550</v>
-      </c>
-      <c r="L25" s="5">
-        <v>0</v>
-      </c>
-      <c r="M25" s="5"/>
+        <v>50</v>
+      </c>
+      <c r="K25" s="5"/>
+      <c r="L25" s="5"/>
+      <c r="M25" s="5" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="26" ht="28" customHeight="true" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
         <v>38</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="C26" s="5">
-        <v>3000</v>
+        <v>5000</v>
       </c>
       <c r="D26" s="5">
         <v>600</v>
       </c>
       <c r="E26" s="5">
-        <v>1000</v>
+        <v>1200</v>
       </c>
       <c r="F26" s="5">
-        <v>150</v>
+        <v>200</v>
       </c>
       <c r="G26" s="5" t="b">
         <v>1</v>
@@ -1290,13 +1292,13 @@
         <v>90</v>
       </c>
       <c r="I26" s="5">
-        <v>200</v>
+        <v>300</v>
       </c>
       <c r="J26" s="5">
         <v>60</v>
       </c>
       <c r="K26" s="5">
-        <v>250</v>
+        <v>400</v>
       </c>
       <c r="L26" s="5">
         <v>600</v>
@@ -1308,22 +1310,22 @@
         <v>39</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="C27" s="5">
-        <v>3000</v>
+        <v>5000</v>
       </c>
       <c r="D27" s="5">
-        <v>1005</v>
+        <v>900</v>
       </c>
       <c r="E27" s="5">
-        <v>1400</v>
+        <v>1000</v>
       </c>
       <c r="F27" s="5">
         <v>100</v>
       </c>
       <c r="G27" s="5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H27" s="5">
         <v>90</v>
@@ -1332,44 +1334,92 @@
         <v>250</v>
       </c>
       <c r="J27" s="5">
+        <v>0</v>
+      </c>
+      <c r="K27" s="5">
+        <v>550</v>
+      </c>
+      <c r="L27" s="5">
+        <v>1100</v>
+      </c>
+      <c r="M27" s="5"/>
+    </row>
+    <row r="28" ht="28" customHeight="true" x14ac:dyDescent="0.25">
+      <c r="A28" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C28" s="5">
+        <v>3000</v>
+      </c>
+      <c r="D28" s="5">
+        <v>600</v>
+      </c>
+      <c r="E28" s="5">
+        <v>1000</v>
+      </c>
+      <c r="F28" s="5">
+        <v>200</v>
+      </c>
+      <c r="G28" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H28" s="5">
+        <v>90</v>
+      </c>
+      <c r="I28" s="5">
+        <v>200</v>
+      </c>
+      <c r="J28" s="5">
         <v>60</v>
       </c>
-      <c r="K27" s="5">
+      <c r="K28" s="5">
+        <v>250</v>
+      </c>
+      <c r="L28" s="5">
+        <v>600</v>
+      </c>
+      <c r="M28" s="5"/>
+    </row>
+    <row r="29" ht="28" customHeight="true" x14ac:dyDescent="0.25">
+      <c r="A29" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C29" s="5">
+        <v>3000</v>
+      </c>
+      <c r="D29" s="5">
+        <v>1005</v>
+      </c>
+      <c r="E29" s="5">
+        <v>1400</v>
+      </c>
+      <c r="F29" s="5">
+        <v>100</v>
+      </c>
+      <c r="G29" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H29" s="5">
+        <v>90</v>
+      </c>
+      <c r="I29" s="5">
+        <v>250</v>
+      </c>
+      <c r="J29" s="5">
+        <v>60</v>
+      </c>
+      <c r="K29" s="5">
         <v>450</v>
       </c>
-      <c r="L27" s="5">
+      <c r="L29" s="5">
         <v>1000</v>
       </c>
-      <c r="M27" s="5"/>
-    </row>
-    <row r="28" ht="28" customHeight="true" x14ac:dyDescent="0.25">
-      <c r="A28" s="5"/>
-      <c r="B28" s="5"/>
-      <c r="C28" s="5"/>
-      <c r="D28" s="5"/>
-      <c r="E28" s="5"/>
-      <c r="F28" s="5"/>
-      <c r="G28" s="5"/>
-      <c r="H28" s="5"/>
-      <c r="I28" s="5"/>
-      <c r="J28" s="5"/>
-      <c r="K28" s="5"/>
-      <c r="L28" s="5"/>
-      <c r="M28" s="5"/>
-    </row>
-    <row r="29" ht="28" customHeight="true" x14ac:dyDescent="0.25">
-      <c r="A29" s="5"/>
-      <c r="B29" s="5"/>
-      <c r="C29" s="5"/>
-      <c r="D29" s="5"/>
-      <c r="E29" s="5"/>
-      <c r="F29" s="5"/>
-      <c r="G29" s="5"/>
-      <c r="H29" s="5"/>
-      <c r="I29" s="5"/>
-      <c r="J29" s="5"/>
-      <c r="K29" s="5"/>
-      <c r="L29" s="5"/>
       <c r="M29" s="5"/>
     </row>
     <row r="30" ht="28" customHeight="true" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
[Feat] (Client) Add HP, MPBar Back To PlayerHUD
</commit_message>
<xml_diff>
--- a/CharacterStats.xlsx
+++ b/CharacterStats.xlsx
@@ -72,31 +72,31 @@
     <t>Normal</t>
   </si>
   <si>
+    <t>Chicken</t>
+  </si>
+  <si>
     <t>YellowBird</t>
   </si>
   <si>
-    <t>Chicken</t>
+    <t>Frog</t>
   </si>
   <si>
     <t>MushRoom</t>
   </si>
   <si>
-    <t>Frog</t>
+    <t>Kabu</t>
   </si>
   <si>
     <t>PurpleBeatle</t>
   </si>
   <si>
-    <t>Kabu</t>
+    <t>NormalBear</t>
   </si>
   <si>
     <t>BossDyna</t>
   </si>
   <si>
     <t>Boss</t>
-  </si>
-  <si>
-    <t>NormalBear</t>
   </si>
   <si>
     <t>Scary</t>
@@ -852,13 +852,13 @@
         <v>100</v>
       </c>
       <c r="G14" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H14" s="5">
         <v>50</v>
       </c>
       <c r="I14" s="5">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="J14" s="5">
         <v>0</v>
@@ -887,13 +887,13 @@
         <v>100</v>
       </c>
       <c r="G15" s="5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H15" s="5">
         <v>50</v>
       </c>
       <c r="I15" s="5">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="J15" s="5">
         <v>0</v>
@@ -907,73 +907,73 @@
         <v>25</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="C16" s="5">
-        <v>5000</v>
+        <v>200</v>
       </c>
       <c r="D16" s="5">
-        <v>1005</v>
+        <v>40</v>
       </c>
       <c r="E16" s="5">
-        <v>1400</v>
+        <v>500</v>
       </c>
       <c r="F16" s="5">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="G16" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H16" s="5">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="I16" s="5">
-        <v>350</v>
+        <v>160</v>
       </c>
       <c r="J16" s="5">
         <v>0</v>
       </c>
-      <c r="K16" s="5">
-        <v>600</v>
-      </c>
-      <c r="L16" s="5">
-        <v>1000</v>
-      </c>
+      <c r="K16" s="5"/>
+      <c r="L16" s="5"/>
       <c r="M16" s="5"/>
     </row>
     <row r="17" ht="28" customHeight="true" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B17" s="5" t="s">
-        <v>18</v>
-      </c>
       <c r="C17" s="5">
-        <v>200</v>
+        <v>5000</v>
       </c>
       <c r="D17" s="5">
-        <v>40</v>
+        <v>1005</v>
       </c>
       <c r="E17" s="5">
-        <v>500</v>
+        <v>1400</v>
       </c>
       <c r="F17" s="5">
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="G17" s="5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H17" s="5">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="I17" s="5">
-        <v>160</v>
+        <v>350</v>
       </c>
       <c r="J17" s="5">
         <v>0</v>
       </c>
-      <c r="K17" s="5"/>
-      <c r="L17" s="5"/>
+      <c r="K17" s="5">
+        <v>600</v>
+      </c>
+      <c r="L17" s="5">
+        <v>1000</v>
+      </c>
       <c r="M17" s="5"/>
     </row>
     <row r="18" ht="28" customHeight="true" x14ac:dyDescent="0.25">
@@ -1271,7 +1271,7 @@
         <v>38</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C26" s="5">
         <v>5000</v>
@@ -1310,7 +1310,7 @@
         <v>39</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C27" s="5">
         <v>5000</v>
@@ -1349,7 +1349,7 @@
         <v>40</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C28" s="5">
         <v>3000</v>
@@ -1388,7 +1388,7 @@
         <v>41</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C29" s="5">
         <v>3000</v>

</xml_diff>

<commit_message>
[Feat] (Client) Create CBossDyna Class Which Represent Final Boss
</commit_message>
<xml_diff>
--- a/CharacterStats.xlsx
+++ b/CharacterStats.xlsx
@@ -72,31 +72,31 @@
     <t>Normal</t>
   </si>
   <si>
+    <t>YellowBird</t>
+  </si>
+  <si>
     <t>Chicken</t>
   </si>
   <si>
-    <t>YellowBird</t>
+    <t>MushRoom</t>
   </si>
   <si>
     <t>Frog</t>
   </si>
   <si>
-    <t>MushRoom</t>
+    <t>PurpleBeatle</t>
   </si>
   <si>
     <t>Kabu</t>
   </si>
   <si>
-    <t>PurpleBeatle</t>
+    <t>BossDyna</t>
+  </si>
+  <si>
+    <t>Boss</t>
   </si>
   <si>
     <t>NormalBear</t>
-  </si>
-  <si>
-    <t>BossDyna</t>
-  </si>
-  <si>
-    <t>Boss</t>
   </si>
   <si>
     <t>Scary</t>
@@ -852,13 +852,13 @@
         <v>100</v>
       </c>
       <c r="G14" s="5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H14" s="5">
         <v>50</v>
       </c>
       <c r="I14" s="5">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="J14" s="5">
         <v>0</v>
@@ -887,13 +887,13 @@
         <v>100</v>
       </c>
       <c r="G15" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H15" s="5">
         <v>50</v>
       </c>
       <c r="I15" s="5">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="J15" s="5">
         <v>0</v>
@@ -907,73 +907,73 @@
         <v>25</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="C16" s="5">
-        <v>200</v>
+        <v>5000</v>
       </c>
       <c r="D16" s="5">
-        <v>40</v>
+        <v>1005</v>
       </c>
       <c r="E16" s="5">
-        <v>500</v>
+        <v>1400</v>
       </c>
       <c r="F16" s="5">
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="G16" s="5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H16" s="5">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="I16" s="5">
-        <v>160</v>
+        <v>350</v>
       </c>
       <c r="J16" s="5">
         <v>0</v>
       </c>
-      <c r="K16" s="5"/>
-      <c r="L16" s="5"/>
+      <c r="K16" s="5">
+        <v>600</v>
+      </c>
+      <c r="L16" s="5">
+        <v>1000</v>
+      </c>
       <c r="M16" s="5"/>
     </row>
     <row r="17" ht="28" customHeight="true" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="C17" s="5">
-        <v>5000</v>
+        <v>200</v>
       </c>
       <c r="D17" s="5">
-        <v>1005</v>
+        <v>40</v>
       </c>
       <c r="E17" s="5">
-        <v>1400</v>
+        <v>500</v>
       </c>
       <c r="F17" s="5">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="G17" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H17" s="5">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="I17" s="5">
-        <v>350</v>
+        <v>160</v>
       </c>
       <c r="J17" s="5">
         <v>0</v>
       </c>
-      <c r="K17" s="5">
-        <v>600</v>
-      </c>
-      <c r="L17" s="5">
-        <v>1000</v>
-      </c>
+      <c r="K17" s="5"/>
+      <c r="L17" s="5"/>
       <c r="M17" s="5"/>
     </row>
     <row r="18" ht="28" customHeight="true" x14ac:dyDescent="0.25">
@@ -1271,7 +1271,7 @@
         <v>38</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C26" s="5">
         <v>5000</v>
@@ -1310,7 +1310,7 @@
         <v>39</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C27" s="5">
         <v>5000</v>
@@ -1349,7 +1349,7 @@
         <v>40</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C28" s="5">
         <v>3000</v>
@@ -1388,7 +1388,7 @@
         <v>41</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C29" s="5">
         <v>3000</v>

</xml_diff>

<commit_message>
[Feat] (Client) BossDyna Head Toggle Up And Down
</commit_message>
<xml_diff>
--- a/CharacterStats.xlsx
+++ b/CharacterStats.xlsx
@@ -72,31 +72,31 @@
     <t>Normal</t>
   </si>
   <si>
+    <t>Chicken</t>
+  </si>
+  <si>
     <t>YellowBird</t>
   </si>
   <si>
-    <t>Chicken</t>
+    <t>Frog</t>
   </si>
   <si>
     <t>MushRoom</t>
   </si>
   <si>
-    <t>Frog</t>
+    <t>Kabu</t>
   </si>
   <si>
     <t>PurpleBeatle</t>
   </si>
   <si>
-    <t>Kabu</t>
+    <t>NormalBear</t>
   </si>
   <si>
     <t>BossDyna</t>
   </si>
   <si>
     <t>Boss</t>
-  </si>
-  <si>
-    <t>NormalBear</t>
   </si>
   <si>
     <t>Scary</t>
@@ -852,13 +852,13 @@
         <v>100</v>
       </c>
       <c r="G14" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H14" s="5">
         <v>50</v>
       </c>
       <c r="I14" s="5">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="J14" s="5">
         <v>0</v>
@@ -887,13 +887,13 @@
         <v>100</v>
       </c>
       <c r="G15" s="5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H15" s="5">
         <v>50</v>
       </c>
       <c r="I15" s="5">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="J15" s="5">
         <v>0</v>
@@ -907,73 +907,73 @@
         <v>25</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="C16" s="5">
-        <v>5000</v>
+        <v>200</v>
       </c>
       <c r="D16" s="5">
-        <v>1005</v>
+        <v>40</v>
       </c>
       <c r="E16" s="5">
-        <v>1400</v>
+        <v>500</v>
       </c>
       <c r="F16" s="5">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="G16" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H16" s="5">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="I16" s="5">
-        <v>350</v>
+        <v>160</v>
       </c>
       <c r="J16" s="5">
         <v>0</v>
       </c>
-      <c r="K16" s="5">
-        <v>600</v>
-      </c>
-      <c r="L16" s="5">
-        <v>1000</v>
-      </c>
+      <c r="K16" s="5"/>
+      <c r="L16" s="5"/>
       <c r="M16" s="5"/>
     </row>
     <row r="17" ht="28" customHeight="true" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B17" s="5" t="s">
-        <v>18</v>
-      </c>
       <c r="C17" s="5">
-        <v>200</v>
+        <v>5000</v>
       </c>
       <c r="D17" s="5">
-        <v>40</v>
+        <v>800</v>
       </c>
       <c r="E17" s="5">
+        <v>1400</v>
+      </c>
+      <c r="F17" s="5">
+        <v>100</v>
+      </c>
+      <c r="G17" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="H17" s="5">
+        <v>90</v>
+      </c>
+      <c r="I17" s="5">
+        <v>350</v>
+      </c>
+      <c r="J17" s="5">
+        <v>0</v>
+      </c>
+      <c r="K17" s="5">
         <v>500</v>
       </c>
-      <c r="F17" s="5">
-        <v>150</v>
-      </c>
-      <c r="G17" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="H17" s="5">
-        <v>80</v>
-      </c>
-      <c r="I17" s="5">
-        <v>160</v>
-      </c>
-      <c r="J17" s="5">
-        <v>0</v>
-      </c>
-      <c r="K17" s="5"/>
-      <c r="L17" s="5"/>
+      <c r="L17" s="5">
+        <v>800</v>
+      </c>
       <c r="M17" s="5"/>
     </row>
     <row r="18" ht="28" customHeight="true" x14ac:dyDescent="0.25">
@@ -1271,7 +1271,7 @@
         <v>38</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C26" s="5">
         <v>5000</v>
@@ -1310,7 +1310,7 @@
         <v>39</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C27" s="5">
         <v>5000</v>
@@ -1349,7 +1349,7 @@
         <v>40</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C28" s="5">
         <v>3000</v>
@@ -1388,7 +1388,7 @@
         <v>41</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C29" s="5">
         <v>3000</v>

</xml_diff>

<commit_message>
[Feat] (Client) Create Far Attack Logic Of BossDyna
</commit_message>
<xml_diff>
--- a/CharacterStats.xlsx
+++ b/CharacterStats.xlsx
@@ -72,31 +72,31 @@
     <t>Normal</t>
   </si>
   <si>
+    <t>YellowBird</t>
+  </si>
+  <si>
     <t>Chicken</t>
   </si>
   <si>
-    <t>YellowBird</t>
+    <t>MushRoom</t>
   </si>
   <si>
     <t>Frog</t>
   </si>
   <si>
-    <t>MushRoom</t>
+    <t>PurpleBeatle</t>
   </si>
   <si>
     <t>Kabu</t>
   </si>
   <si>
-    <t>PurpleBeatle</t>
+    <t>BossDyna</t>
+  </si>
+  <si>
+    <t>Boss</t>
   </si>
   <si>
     <t>NormalBear</t>
-  </si>
-  <si>
-    <t>BossDyna</t>
-  </si>
-  <si>
-    <t>Boss</t>
   </si>
   <si>
     <t>Scary</t>
@@ -852,13 +852,13 @@
         <v>100</v>
       </c>
       <c r="G14" s="5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H14" s="5">
         <v>50</v>
       </c>
       <c r="I14" s="5">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="J14" s="5">
         <v>0</v>
@@ -887,13 +887,13 @@
         <v>100</v>
       </c>
       <c r="G15" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H15" s="5">
         <v>50</v>
       </c>
       <c r="I15" s="5">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="J15" s="5">
         <v>0</v>
@@ -907,73 +907,73 @@
         <v>25</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="C16" s="5">
-        <v>200</v>
+        <v>5000</v>
       </c>
       <c r="D16" s="5">
-        <v>40</v>
+        <v>800</v>
       </c>
       <c r="E16" s="5">
+        <v>1400</v>
+      </c>
+      <c r="F16" s="5">
+        <v>100</v>
+      </c>
+      <c r="G16" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="H16" s="5">
+        <v>90</v>
+      </c>
+      <c r="I16" s="5">
+        <v>350</v>
+      </c>
+      <c r="J16" s="5">
+        <v>0</v>
+      </c>
+      <c r="K16" s="5">
         <v>500</v>
       </c>
-      <c r="F16" s="5">
-        <v>150</v>
-      </c>
-      <c r="G16" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="H16" s="5">
-        <v>80</v>
-      </c>
-      <c r="I16" s="5">
-        <v>160</v>
-      </c>
-      <c r="J16" s="5">
-        <v>0</v>
-      </c>
-      <c r="K16" s="5"/>
-      <c r="L16" s="5"/>
+      <c r="L16" s="5">
+        <v>800</v>
+      </c>
       <c r="M16" s="5"/>
     </row>
     <row r="17" ht="28" customHeight="true" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="C17" s="5">
-        <v>5000</v>
+        <v>200</v>
       </c>
       <c r="D17" s="5">
-        <v>800</v>
+        <v>40</v>
       </c>
       <c r="E17" s="5">
-        <v>1400</v>
+        <v>500</v>
       </c>
       <c r="F17" s="5">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="G17" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H17" s="5">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="I17" s="5">
-        <v>350</v>
+        <v>160</v>
       </c>
       <c r="J17" s="5">
         <v>0</v>
       </c>
-      <c r="K17" s="5">
-        <v>500</v>
-      </c>
-      <c r="L17" s="5">
-        <v>800</v>
-      </c>
+      <c r="K17" s="5"/>
+      <c r="L17" s="5"/>
       <c r="M17" s="5"/>
     </row>
     <row r="18" ht="28" customHeight="true" x14ac:dyDescent="0.25">
@@ -1271,7 +1271,7 @@
         <v>38</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C26" s="5">
         <v>5000</v>
@@ -1310,7 +1310,7 @@
         <v>39</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C27" s="5">
         <v>5000</v>
@@ -1349,7 +1349,7 @@
         <v>40</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C28" s="5">
         <v>3000</v>
@@ -1388,7 +1388,7 @@
         <v>41</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C29" s="5">
         <v>3000</v>

</xml_diff>

<commit_message>
[Feat] (Client) Create UpdateMovement Function In BossDyna Monster & Randomly And Freely Move Boss Dyna
</commit_message>
<xml_diff>
--- a/CharacterStats.xlsx
+++ b/CharacterStats.xlsx
@@ -72,31 +72,31 @@
     <t>Normal</t>
   </si>
   <si>
+    <t>Chicken</t>
+  </si>
+  <si>
     <t>YellowBird</t>
   </si>
   <si>
-    <t>Chicken</t>
+    <t>Frog</t>
   </si>
   <si>
     <t>MushRoom</t>
   </si>
   <si>
-    <t>Frog</t>
+    <t>Kabu</t>
   </si>
   <si>
     <t>PurpleBeatle</t>
   </si>
   <si>
-    <t>Kabu</t>
+    <t>NormalBear</t>
   </si>
   <si>
     <t>BossDyna</t>
   </si>
   <si>
     <t>Boss</t>
-  </si>
-  <si>
-    <t>NormalBear</t>
   </si>
   <si>
     <t>Scary</t>
@@ -852,13 +852,13 @@
         <v>100</v>
       </c>
       <c r="G14" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H14" s="5">
         <v>50</v>
       </c>
       <c r="I14" s="5">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="J14" s="5">
         <v>0</v>
@@ -887,13 +887,13 @@
         <v>100</v>
       </c>
       <c r="G15" s="5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H15" s="5">
         <v>50</v>
       </c>
       <c r="I15" s="5">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="J15" s="5">
         <v>0</v>
@@ -907,73 +907,73 @@
         <v>25</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="C16" s="5">
-        <v>5000</v>
+        <v>200</v>
       </c>
       <c r="D16" s="5">
-        <v>800</v>
+        <v>40</v>
       </c>
       <c r="E16" s="5">
-        <v>1400</v>
+        <v>500</v>
       </c>
       <c r="F16" s="5">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="G16" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H16" s="5">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="I16" s="5">
-        <v>350</v>
+        <v>160</v>
       </c>
       <c r="J16" s="5">
         <v>0</v>
       </c>
-      <c r="K16" s="5">
-        <v>500</v>
-      </c>
-      <c r="L16" s="5">
-        <v>800</v>
-      </c>
+      <c r="K16" s="5"/>
+      <c r="L16" s="5"/>
       <c r="M16" s="5"/>
     </row>
     <row r="17" ht="28" customHeight="true" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B17" s="5" t="s">
-        <v>18</v>
-      </c>
       <c r="C17" s="5">
-        <v>200</v>
+        <v>5000</v>
       </c>
       <c r="D17" s="5">
-        <v>40</v>
+        <v>800</v>
       </c>
       <c r="E17" s="5">
+        <v>1400</v>
+      </c>
+      <c r="F17" s="5">
+        <v>100</v>
+      </c>
+      <c r="G17" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="H17" s="5">
+        <v>90</v>
+      </c>
+      <c r="I17" s="5">
+        <v>350</v>
+      </c>
+      <c r="J17" s="5">
+        <v>0</v>
+      </c>
+      <c r="K17" s="5">
         <v>500</v>
       </c>
-      <c r="F17" s="5">
-        <v>150</v>
-      </c>
-      <c r="G17" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="H17" s="5">
-        <v>80</v>
-      </c>
-      <c r="I17" s="5">
-        <v>160</v>
-      </c>
-      <c r="J17" s="5">
-        <v>0</v>
-      </c>
-      <c r="K17" s="5"/>
-      <c r="L17" s="5"/>
+      <c r="L17" s="5">
+        <v>800</v>
+      </c>
       <c r="M17" s="5"/>
     </row>
     <row r="18" ht="28" customHeight="true" x14ac:dyDescent="0.25">
@@ -1271,7 +1271,7 @@
         <v>38</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C26" s="5">
         <v>5000</v>
@@ -1310,7 +1310,7 @@
         <v>39</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C27" s="5">
         <v>5000</v>
@@ -1349,7 +1349,7 @@
         <v>40</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C28" s="5">
         <v>3000</v>
@@ -1388,7 +1388,7 @@
         <v>41</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C29" s="5">
         <v>3000</v>

</xml_diff>

<commit_message>
[Feat] (Client) Create UpdateAppearance Function In BossDyna & Make Appear Effect In the Beginning
</commit_message>
<xml_diff>
--- a/CharacterStats.xlsx
+++ b/CharacterStats.xlsx
@@ -948,7 +948,7 @@
         <v>5000</v>
       </c>
       <c r="D17" s="5">
-        <v>800</v>
+        <v>650</v>
       </c>
       <c r="E17" s="5">
         <v>1400</v>
@@ -960,7 +960,7 @@
         <v>0</v>
       </c>
       <c r="H17" s="5">
-        <v>90</v>
+        <v>10</v>
       </c>
       <c r="I17" s="5">
         <v>350</v>
@@ -969,10 +969,10 @@
         <v>0</v>
       </c>
       <c r="K17" s="5">
-        <v>500</v>
+        <v>400</v>
       </c>
       <c r="L17" s="5">
-        <v>800</v>
+        <v>650</v>
       </c>
       <c r="M17" s="5"/>
     </row>

</xml_diff>

<commit_message>
[Fix] (Client) Player World Pos Set Right When It Goes More Left Then Boss World Resolution
</commit_message>
<xml_diff>
--- a/CharacterStats.xlsx
+++ b/CharacterStats.xlsx
@@ -72,31 +72,31 @@
     <t>Normal</t>
   </si>
   <si>
+    <t>YellowBird</t>
+  </si>
+  <si>
     <t>Chicken</t>
   </si>
   <si>
-    <t>YellowBird</t>
+    <t>MushRoom</t>
   </si>
   <si>
     <t>Frog</t>
   </si>
   <si>
-    <t>MushRoom</t>
+    <t>PurpleBeatle</t>
   </si>
   <si>
     <t>Kabu</t>
   </si>
   <si>
-    <t>PurpleBeatle</t>
+    <t>BossDyna</t>
+  </si>
+  <si>
+    <t>Boss</t>
   </si>
   <si>
     <t>NormalBear</t>
-  </si>
-  <si>
-    <t>BossDyna</t>
-  </si>
-  <si>
-    <t>Boss</t>
   </si>
   <si>
     <t>Scary</t>
@@ -852,13 +852,13 @@
         <v>100</v>
       </c>
       <c r="G14" s="5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H14" s="5">
         <v>50</v>
       </c>
       <c r="I14" s="5">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="J14" s="5">
         <v>0</v>
@@ -887,13 +887,13 @@
         <v>100</v>
       </c>
       <c r="G15" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H15" s="5">
         <v>50</v>
       </c>
       <c r="I15" s="5">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="J15" s="5">
         <v>0</v>
@@ -907,73 +907,73 @@
         <v>25</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="C16" s="5">
-        <v>200</v>
+        <v>5000</v>
       </c>
       <c r="D16" s="5">
-        <v>40</v>
+        <v>650</v>
       </c>
       <c r="E16" s="5">
-        <v>500</v>
+        <v>1400</v>
       </c>
       <c r="F16" s="5">
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="G16" s="5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H16" s="5">
-        <v>80</v>
+        <v>10</v>
       </c>
       <c r="I16" s="5">
-        <v>160</v>
+        <v>350</v>
       </c>
       <c r="J16" s="5">
         <v>0</v>
       </c>
-      <c r="K16" s="5"/>
-      <c r="L16" s="5"/>
+      <c r="K16" s="5">
+        <v>400</v>
+      </c>
+      <c r="L16" s="5">
+        <v>650</v>
+      </c>
       <c r="M16" s="5"/>
     </row>
     <row r="17" ht="28" customHeight="true" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="C17" s="5">
-        <v>5000</v>
+        <v>200</v>
       </c>
       <c r="D17" s="5">
-        <v>650</v>
+        <v>40</v>
       </c>
       <c r="E17" s="5">
-        <v>1400</v>
+        <v>500</v>
       </c>
       <c r="F17" s="5">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="G17" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H17" s="5">
-        <v>10</v>
+        <v>80</v>
       </c>
       <c r="I17" s="5">
-        <v>350</v>
+        <v>160</v>
       </c>
       <c r="J17" s="5">
         <v>0</v>
       </c>
-      <c r="K17" s="5">
-        <v>400</v>
-      </c>
-      <c r="L17" s="5">
-        <v>650</v>
-      </c>
+      <c r="K17" s="5"/>
+      <c r="L17" s="5"/>
       <c r="M17" s="5"/>
     </row>
     <row r="18" ht="28" customHeight="true" x14ac:dyDescent="0.25">
@@ -1271,7 +1271,7 @@
         <v>38</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C26" s="5">
         <v>5000</v>
@@ -1310,7 +1310,7 @@
         <v>39</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C27" s="5">
         <v>5000</v>
@@ -1349,7 +1349,7 @@
         <v>40</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C28" s="5">
         <v>3000</v>
@@ -1388,7 +1388,7 @@
         <v>41</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C29" s="5">
         <v>3000</v>

</xml_diff>

<commit_message>
[Feat] (Client) MakeBossAngry Virtual Function In BossMonster & Make Base Color More Red
</commit_message>
<xml_diff>
--- a/CharacterStats.xlsx
+++ b/CharacterStats.xlsx
@@ -72,31 +72,31 @@
     <t>Normal</t>
   </si>
   <si>
+    <t>Chicken</t>
+  </si>
+  <si>
     <t>YellowBird</t>
   </si>
   <si>
-    <t>Chicken</t>
+    <t>Frog</t>
   </si>
   <si>
     <t>MushRoom</t>
   </si>
   <si>
-    <t>Frog</t>
+    <t>Kabu</t>
   </si>
   <si>
     <t>PurpleBeatle</t>
   </si>
   <si>
-    <t>Kabu</t>
+    <t>NormalBear</t>
   </si>
   <si>
     <t>BossDyna</t>
   </si>
   <si>
     <t>Boss</t>
-  </si>
-  <si>
-    <t>NormalBear</t>
   </si>
   <si>
     <t>Scary</t>
@@ -852,13 +852,13 @@
         <v>100</v>
       </c>
       <c r="G14" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H14" s="5">
         <v>50</v>
       </c>
       <c r="I14" s="5">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="J14" s="5">
         <v>0</v>
@@ -887,13 +887,13 @@
         <v>100</v>
       </c>
       <c r="G15" s="5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H15" s="5">
         <v>50</v>
       </c>
       <c r="I15" s="5">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="J15" s="5">
         <v>0</v>
@@ -907,73 +907,73 @@
         <v>25</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="C16" s="5">
-        <v>5000</v>
+        <v>200</v>
       </c>
       <c r="D16" s="5">
-        <v>650</v>
+        <v>40</v>
       </c>
       <c r="E16" s="5">
-        <v>1400</v>
+        <v>500</v>
       </c>
       <c r="F16" s="5">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="G16" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H16" s="5">
-        <v>10</v>
+        <v>80</v>
       </c>
       <c r="I16" s="5">
-        <v>350</v>
+        <v>160</v>
       </c>
       <c r="J16" s="5">
         <v>0</v>
       </c>
-      <c r="K16" s="5">
-        <v>400</v>
-      </c>
-      <c r="L16" s="5">
-        <v>650</v>
-      </c>
+      <c r="K16" s="5"/>
+      <c r="L16" s="5"/>
       <c r="M16" s="5"/>
     </row>
     <row r="17" ht="28" customHeight="true" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B17" s="5" t="s">
-        <v>18</v>
-      </c>
       <c r="C17" s="5">
-        <v>200</v>
+        <v>5000</v>
       </c>
       <c r="D17" s="5">
-        <v>40</v>
+        <v>650</v>
       </c>
       <c r="E17" s="5">
-        <v>500</v>
+        <v>1400</v>
       </c>
       <c r="F17" s="5">
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="G17" s="5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H17" s="5">
-        <v>80</v>
+        <v>10</v>
       </c>
       <c r="I17" s="5">
-        <v>160</v>
+        <v>350</v>
       </c>
       <c r="J17" s="5">
         <v>0</v>
       </c>
-      <c r="K17" s="5"/>
-      <c r="L17" s="5"/>
+      <c r="K17" s="5">
+        <v>400</v>
+      </c>
+      <c r="L17" s="5">
+        <v>650</v>
+      </c>
       <c r="M17" s="5"/>
     </row>
     <row r="18" ht="28" customHeight="true" x14ac:dyDescent="0.25">
@@ -1271,7 +1271,7 @@
         <v>38</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C26" s="5">
         <v>5000</v>
@@ -1310,7 +1310,7 @@
         <v>39</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C27" s="5">
         <v>5000</v>
@@ -1349,7 +1349,7 @@
         <v>40</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C28" s="5">
         <v>3000</v>
@@ -1388,7 +1388,7 @@
         <v>41</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C29" s="5">
         <v>3000</v>

</xml_diff>

<commit_message>
[Feat] (Client) Make Boss Particle Object & Boss Make Particle Periodically
</commit_message>
<xml_diff>
--- a/CharacterStats.xlsx
+++ b/CharacterStats.xlsx
@@ -72,31 +72,31 @@
     <t>Normal</t>
   </si>
   <si>
+    <t>YellowBird</t>
+  </si>
+  <si>
     <t>Chicken</t>
   </si>
   <si>
-    <t>YellowBird</t>
+    <t>MushRoom</t>
   </si>
   <si>
     <t>Frog</t>
   </si>
   <si>
-    <t>MushRoom</t>
+    <t>PurpleBeatle</t>
   </si>
   <si>
     <t>Kabu</t>
   </si>
   <si>
-    <t>PurpleBeatle</t>
+    <t>BossDyna</t>
+  </si>
+  <si>
+    <t>Boss</t>
   </si>
   <si>
     <t>NormalBear</t>
-  </si>
-  <si>
-    <t>BossDyna</t>
-  </si>
-  <si>
-    <t>Boss</t>
   </si>
   <si>
     <t>Scary</t>
@@ -852,13 +852,13 @@
         <v>100</v>
       </c>
       <c r="G14" s="5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H14" s="5">
         <v>50</v>
       </c>
       <c r="I14" s="5">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="J14" s="5">
         <v>0</v>
@@ -887,13 +887,13 @@
         <v>100</v>
       </c>
       <c r="G15" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H15" s="5">
         <v>50</v>
       </c>
       <c r="I15" s="5">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="J15" s="5">
         <v>0</v>
@@ -907,73 +907,73 @@
         <v>25</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="C16" s="5">
-        <v>200</v>
+        <v>5000</v>
       </c>
       <c r="D16" s="5">
-        <v>40</v>
+        <v>650</v>
       </c>
       <c r="E16" s="5">
-        <v>500</v>
+        <v>1400</v>
       </c>
       <c r="F16" s="5">
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="G16" s="5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H16" s="5">
-        <v>80</v>
+        <v>10</v>
       </c>
       <c r="I16" s="5">
-        <v>160</v>
+        <v>350</v>
       </c>
       <c r="J16" s="5">
         <v>0</v>
       </c>
-      <c r="K16" s="5"/>
-      <c r="L16" s="5"/>
+      <c r="K16" s="5">
+        <v>400</v>
+      </c>
+      <c r="L16" s="5">
+        <v>650</v>
+      </c>
       <c r="M16" s="5"/>
     </row>
     <row r="17" ht="28" customHeight="true" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="C17" s="5">
-        <v>5000</v>
+        <v>200</v>
       </c>
       <c r="D17" s="5">
-        <v>650</v>
+        <v>40</v>
       </c>
       <c r="E17" s="5">
-        <v>1400</v>
+        <v>500</v>
       </c>
       <c r="F17" s="5">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="G17" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H17" s="5">
-        <v>10</v>
+        <v>80</v>
       </c>
       <c r="I17" s="5">
-        <v>350</v>
+        <v>160</v>
       </c>
       <c r="J17" s="5">
         <v>0</v>
       </c>
-      <c r="K17" s="5">
-        <v>400</v>
-      </c>
-      <c r="L17" s="5">
-        <v>650</v>
-      </c>
+      <c r="K17" s="5"/>
+      <c r="L17" s="5"/>
       <c r="M17" s="5"/>
     </row>
     <row r="18" ht="28" customHeight="true" x14ac:dyDescent="0.25">
@@ -1271,7 +1271,7 @@
         <v>38</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C26" s="5">
         <v>5000</v>
@@ -1310,7 +1310,7 @@
         <v>39</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C27" s="5">
         <v>5000</v>
@@ -1349,7 +1349,7 @@
         <v>40</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C28" s="5">
         <v>3000</v>
@@ -1388,7 +1388,7 @@
         <v>41</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C29" s="5">
         <v>3000</v>

</xml_diff>

<commit_message>
[Feat] (Client) Set std::mt19937 Memeber Variable In Client Manager & Generate Random Number Using Random Library
</commit_message>
<xml_diff>
--- a/CharacterStats.xlsx
+++ b/CharacterStats.xlsx
@@ -72,31 +72,31 @@
     <t>Normal</t>
   </si>
   <si>
+    <t>Chicken</t>
+  </si>
+  <si>
     <t>YellowBird</t>
   </si>
   <si>
-    <t>Chicken</t>
+    <t>Frog</t>
   </si>
   <si>
     <t>MushRoom</t>
   </si>
   <si>
-    <t>Frog</t>
+    <t>Kabu</t>
   </si>
   <si>
     <t>PurpleBeatle</t>
   </si>
   <si>
-    <t>Kabu</t>
+    <t>NormalBear</t>
   </si>
   <si>
     <t>BossDyna</t>
   </si>
   <si>
     <t>Boss</t>
-  </si>
-  <si>
-    <t>NormalBear</t>
   </si>
   <si>
     <t>Scary</t>
@@ -852,13 +852,13 @@
         <v>100</v>
       </c>
       <c r="G14" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H14" s="5">
         <v>50</v>
       </c>
       <c r="I14" s="5">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="J14" s="5">
         <v>0</v>
@@ -887,13 +887,13 @@
         <v>100</v>
       </c>
       <c r="G15" s="5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H15" s="5">
         <v>50</v>
       </c>
       <c r="I15" s="5">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="J15" s="5">
         <v>0</v>
@@ -907,73 +907,73 @@
         <v>25</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="C16" s="5">
-        <v>5000</v>
+        <v>200</v>
       </c>
       <c r="D16" s="5">
-        <v>650</v>
+        <v>40</v>
       </c>
       <c r="E16" s="5">
-        <v>1400</v>
+        <v>500</v>
       </c>
       <c r="F16" s="5">
-        <v>100</v>
+        <v>120</v>
       </c>
       <c r="G16" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H16" s="5">
-        <v>10</v>
+        <v>80</v>
       </c>
       <c r="I16" s="5">
-        <v>350</v>
+        <v>160</v>
       </c>
       <c r="J16" s="5">
         <v>0</v>
       </c>
-      <c r="K16" s="5">
-        <v>400</v>
-      </c>
-      <c r="L16" s="5">
-        <v>650</v>
-      </c>
+      <c r="K16" s="5"/>
+      <c r="L16" s="5"/>
       <c r="M16" s="5"/>
     </row>
     <row r="17" ht="28" customHeight="true" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B17" s="5" t="s">
-        <v>18</v>
-      </c>
       <c r="C17" s="5">
-        <v>200</v>
+        <v>3000</v>
       </c>
       <c r="D17" s="5">
-        <v>40</v>
+        <v>650</v>
       </c>
       <c r="E17" s="5">
-        <v>500</v>
+        <v>1400</v>
       </c>
       <c r="F17" s="5">
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="G17" s="5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H17" s="5">
-        <v>80</v>
+        <v>10</v>
       </c>
       <c r="I17" s="5">
-        <v>160</v>
+        <v>350</v>
       </c>
       <c r="J17" s="5">
         <v>0</v>
       </c>
-      <c r="K17" s="5"/>
-      <c r="L17" s="5"/>
+      <c r="K17" s="5">
+        <v>400</v>
+      </c>
+      <c r="L17" s="5">
+        <v>650</v>
+      </c>
       <c r="M17" s="5"/>
     </row>
     <row r="18" ht="28" customHeight="true" x14ac:dyDescent="0.25">
@@ -1271,10 +1271,10 @@
         <v>38</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C26" s="5">
-        <v>5000</v>
+        <v>2500</v>
       </c>
       <c r="D26" s="5">
         <v>600</v>
@@ -1310,10 +1310,10 @@
         <v>39</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C27" s="5">
-        <v>5000</v>
+        <v>2500</v>
       </c>
       <c r="D27" s="5">
         <v>900</v>
@@ -1349,10 +1349,10 @@
         <v>40</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C28" s="5">
-        <v>3000</v>
+        <v>1500</v>
       </c>
       <c r="D28" s="5">
         <v>600</v>
@@ -1388,10 +1388,10 @@
         <v>41</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C29" s="5">
-        <v>3000</v>
+        <v>2000</v>
       </c>
       <c r="D29" s="5">
         <v>1005</v>

</xml_diff>

<commit_message>
[Feat] (Client) Generage FireBackEffect When PlayerAttack Collider With Monster With World Pos Set In The Middle
</commit_message>
<xml_diff>
--- a/CharacterStats.xlsx
+++ b/CharacterStats.xlsx
@@ -72,31 +72,31 @@
     <t>Normal</t>
   </si>
   <si>
+    <t>YellowBird</t>
+  </si>
+  <si>
     <t>Chicken</t>
   </si>
   <si>
-    <t>YellowBird</t>
+    <t>MushRoom</t>
   </si>
   <si>
     <t>Frog</t>
   </si>
   <si>
-    <t>MushRoom</t>
+    <t>PurpleBeatle</t>
   </si>
   <si>
     <t>Kabu</t>
   </si>
   <si>
-    <t>PurpleBeatle</t>
+    <t>BossDyna</t>
+  </si>
+  <si>
+    <t>Boss</t>
   </si>
   <si>
     <t>NormalBear</t>
-  </si>
-  <si>
-    <t>BossDyna</t>
-  </si>
-  <si>
-    <t>Boss</t>
   </si>
   <si>
     <t>Scary</t>
@@ -852,13 +852,13 @@
         <v>100</v>
       </c>
       <c r="G14" s="5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H14" s="5">
         <v>50</v>
       </c>
       <c r="I14" s="5">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="J14" s="5">
         <v>0</v>
@@ -887,13 +887,13 @@
         <v>100</v>
       </c>
       <c r="G15" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H15" s="5">
         <v>50</v>
       </c>
       <c r="I15" s="5">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="J15" s="5">
         <v>0</v>
@@ -907,73 +907,73 @@
         <v>25</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="C16" s="5">
-        <v>200</v>
+        <v>3000</v>
       </c>
       <c r="D16" s="5">
-        <v>40</v>
+        <v>650</v>
       </c>
       <c r="E16" s="5">
-        <v>500</v>
+        <v>1400</v>
       </c>
       <c r="F16" s="5">
-        <v>120</v>
+        <v>100</v>
       </c>
       <c r="G16" s="5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H16" s="5">
-        <v>80</v>
+        <v>10</v>
       </c>
       <c r="I16" s="5">
-        <v>160</v>
+        <v>350</v>
       </c>
       <c r="J16" s="5">
         <v>0</v>
       </c>
-      <c r="K16" s="5"/>
-      <c r="L16" s="5"/>
+      <c r="K16" s="5">
+        <v>400</v>
+      </c>
+      <c r="L16" s="5">
+        <v>650</v>
+      </c>
       <c r="M16" s="5"/>
     </row>
     <row r="17" ht="28" customHeight="true" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="C17" s="5">
-        <v>3000</v>
+        <v>200</v>
       </c>
       <c r="D17" s="5">
-        <v>650</v>
+        <v>40</v>
       </c>
       <c r="E17" s="5">
-        <v>1400</v>
+        <v>500</v>
       </c>
       <c r="F17" s="5">
-        <v>100</v>
+        <v>120</v>
       </c>
       <c r="G17" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H17" s="5">
-        <v>10</v>
+        <v>80</v>
       </c>
       <c r="I17" s="5">
-        <v>350</v>
+        <v>160</v>
       </c>
       <c r="J17" s="5">
         <v>0</v>
       </c>
-      <c r="K17" s="5">
-        <v>400</v>
-      </c>
-      <c r="L17" s="5">
-        <v>650</v>
-      </c>
+      <c r="K17" s="5"/>
+      <c r="L17" s="5"/>
       <c r="M17" s="5"/>
     </row>
     <row r="18" ht="28" customHeight="true" x14ac:dyDescent="0.25">
@@ -1271,7 +1271,7 @@
         <v>38</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C26" s="5">
         <v>2500</v>
@@ -1310,7 +1310,7 @@
         <v>39</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C27" s="5">
         <v>2500</v>
@@ -1349,7 +1349,7 @@
         <v>40</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C28" s="5">
         <v>1500</v>
@@ -1388,7 +1388,7 @@
         <v>41</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C29" s="5">
         <v>2000</v>

</xml_diff>

<commit_message>
[Feat] (Client) Create BossDynaBaby List In BossDyna Class & Add BossDyna Baby To This List Every Time Boss Dyna Baby Is Made & Destroy All Boss Dyna Baby In The Scene When Boss Dyna Dies
</commit_message>
<xml_diff>
--- a/CharacterStats.xlsx
+++ b/CharacterStats.xlsx
@@ -72,31 +72,31 @@
     <t>Normal</t>
   </si>
   <si>
+    <t>Chicken</t>
+  </si>
+  <si>
     <t>YellowBird</t>
   </si>
   <si>
-    <t>Chicken</t>
+    <t>Frog</t>
   </si>
   <si>
     <t>MushRoom</t>
   </si>
   <si>
-    <t>Frog</t>
+    <t>Kabu</t>
   </si>
   <si>
     <t>PurpleBeatle</t>
   </si>
   <si>
-    <t>Kabu</t>
+    <t>NormalBear</t>
   </si>
   <si>
     <t>BossDyna</t>
   </si>
   <si>
     <t>Boss</t>
-  </si>
-  <si>
-    <t>NormalBear</t>
   </si>
   <si>
     <t>Scary</t>
@@ -852,13 +852,13 @@
         <v>100</v>
       </c>
       <c r="G14" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H14" s="5">
         <v>50</v>
       </c>
       <c r="I14" s="5">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="J14" s="5">
         <v>0</v>
@@ -887,13 +887,13 @@
         <v>100</v>
       </c>
       <c r="G15" s="5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H15" s="5">
         <v>50</v>
       </c>
       <c r="I15" s="5">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="J15" s="5">
         <v>0</v>
@@ -907,73 +907,73 @@
         <v>25</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="C16" s="5">
-        <v>3000</v>
+        <v>200</v>
       </c>
       <c r="D16" s="5">
-        <v>650</v>
+        <v>40</v>
       </c>
       <c r="E16" s="5">
-        <v>1400</v>
+        <v>500</v>
       </c>
       <c r="F16" s="5">
-        <v>100</v>
+        <v>120</v>
       </c>
       <c r="G16" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H16" s="5">
-        <v>10</v>
+        <v>80</v>
       </c>
       <c r="I16" s="5">
-        <v>350</v>
+        <v>160</v>
       </c>
       <c r="J16" s="5">
         <v>0</v>
       </c>
-      <c r="K16" s="5">
-        <v>400</v>
-      </c>
-      <c r="L16" s="5">
-        <v>650</v>
-      </c>
+      <c r="K16" s="5"/>
+      <c r="L16" s="5"/>
       <c r="M16" s="5"/>
     </row>
     <row r="17" ht="28" customHeight="true" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B17" s="5" t="s">
-        <v>18</v>
-      </c>
       <c r="C17" s="5">
-        <v>200</v>
+        <v>3000</v>
       </c>
       <c r="D17" s="5">
-        <v>40</v>
+        <v>650</v>
       </c>
       <c r="E17" s="5">
-        <v>500</v>
+        <v>1400</v>
       </c>
       <c r="F17" s="5">
-        <v>120</v>
+        <v>100</v>
       </c>
       <c r="G17" s="5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H17" s="5">
-        <v>80</v>
+        <v>10</v>
       </c>
       <c r="I17" s="5">
-        <v>160</v>
+        <v>350</v>
       </c>
       <c r="J17" s="5">
         <v>0</v>
       </c>
-      <c r="K17" s="5"/>
-      <c r="L17" s="5"/>
+      <c r="K17" s="5">
+        <v>400</v>
+      </c>
+      <c r="L17" s="5">
+        <v>650</v>
+      </c>
       <c r="M17" s="5"/>
     </row>
     <row r="18" ht="28" customHeight="true" x14ac:dyDescent="0.25">
@@ -1271,7 +1271,7 @@
         <v>38</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C26" s="5">
         <v>2500</v>
@@ -1310,7 +1310,7 @@
         <v>39</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C27" s="5">
         <v>2500</v>
@@ -1349,7 +1349,7 @@
         <v>40</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C28" s="5">
         <v>1500</v>
@@ -1388,7 +1388,7 @@
         <v>41</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C29" s="5">
         <v>2000</v>

</xml_diff>

<commit_message>
[Engine] (Client) Apply Alpha Blend To TileEmptyComponent In TileEmptyComponent::Start Function
</commit_message>
<xml_diff>
--- a/CharacterStats.xlsx
+++ b/CharacterStats.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="64" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="63" uniqueCount="42">
   <si>
     <t>Created by LibXL trial version 4.0.3. Please buy the LibXL full version for removing this message.</t>
   </si>
@@ -72,31 +72,31 @@
     <t>Normal</t>
   </si>
   <si>
+    <t>YellowBird</t>
+  </si>
+  <si>
     <t>Chicken</t>
   </si>
   <si>
-    <t>YellowBird</t>
+    <t>MushRoom</t>
   </si>
   <si>
     <t>Frog</t>
   </si>
   <si>
-    <t>MushRoom</t>
+    <t>PurpleBeatle</t>
   </si>
   <si>
     <t>Kabu</t>
   </si>
   <si>
-    <t>PurpleBeatle</t>
+    <t>BossDyna</t>
+  </si>
+  <si>
+    <t>Boss</t>
   </si>
   <si>
     <t>NormalBear</t>
-  </si>
-  <si>
-    <t>BossDyna</t>
-  </si>
-  <si>
-    <t>Boss</t>
   </si>
   <si>
     <t>Scary</t>
@@ -852,13 +852,13 @@
         <v>100</v>
       </c>
       <c r="G14" s="5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H14" s="5">
         <v>50</v>
       </c>
       <c r="I14" s="5">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="J14" s="5">
         <v>0</v>
@@ -887,13 +887,13 @@
         <v>100</v>
       </c>
       <c r="G15" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H15" s="5">
         <v>50</v>
       </c>
       <c r="I15" s="5">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="J15" s="5">
         <v>0</v>
@@ -907,73 +907,73 @@
         <v>25</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="C16" s="5">
-        <v>200</v>
+        <v>3000</v>
       </c>
       <c r="D16" s="5">
-        <v>40</v>
+        <v>650</v>
       </c>
       <c r="E16" s="5">
-        <v>500</v>
+        <v>1400</v>
       </c>
       <c r="F16" s="5">
-        <v>120</v>
+        <v>100</v>
       </c>
       <c r="G16" s="5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H16" s="5">
-        <v>80</v>
+        <v>10</v>
       </c>
       <c r="I16" s="5">
-        <v>160</v>
+        <v>350</v>
       </c>
       <c r="J16" s="5">
         <v>0</v>
       </c>
-      <c r="K16" s="5"/>
-      <c r="L16" s="5"/>
+      <c r="K16" s="5">
+        <v>400</v>
+      </c>
+      <c r="L16" s="5">
+        <v>650</v>
+      </c>
       <c r="M16" s="5"/>
     </row>
     <row r="17" ht="28" customHeight="true" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="C17" s="5">
-        <v>3000</v>
+        <v>200</v>
       </c>
       <c r="D17" s="5">
-        <v>650</v>
+        <v>40</v>
       </c>
       <c r="E17" s="5">
-        <v>1400</v>
+        <v>500</v>
       </c>
       <c r="F17" s="5">
-        <v>100</v>
+        <v>120</v>
       </c>
       <c r="G17" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H17" s="5">
-        <v>10</v>
+        <v>80</v>
       </c>
       <c r="I17" s="5">
-        <v>350</v>
+        <v>160</v>
       </c>
       <c r="J17" s="5">
         <v>0</v>
       </c>
-      <c r="K17" s="5">
-        <v>400</v>
-      </c>
-      <c r="L17" s="5">
-        <v>650</v>
-      </c>
+      <c r="K17" s="5"/>
+      <c r="L17" s="5"/>
       <c r="M17" s="5"/>
     </row>
     <row r="18" ht="28" customHeight="true" x14ac:dyDescent="0.25">
@@ -1160,7 +1160,7 @@
         <v>35</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="C23" s="5">
         <v>300</v>
@@ -1186,11 +1186,13 @@
       <c r="J23" s="5">
         <v>0</v>
       </c>
-      <c r="K23" s="5"/>
-      <c r="L23" s="5"/>
-      <c r="M23" s="5" t="s">
-        <v>35</v>
-      </c>
+      <c r="K23" s="5">
+        <v>0</v>
+      </c>
+      <c r="L23" s="5">
+        <v>0</v>
+      </c>
+      <c r="M23" s="5"/>
     </row>
     <row r="24" ht="28" customHeight="true" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
@@ -1271,7 +1273,7 @@
         <v>38</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C26" s="5">
         <v>2500</v>
@@ -1310,7 +1312,7 @@
         <v>39</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C27" s="5">
         <v>2500</v>
@@ -1349,7 +1351,7 @@
         <v>40</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C28" s="5">
         <v>1500</v>
@@ -1370,7 +1372,7 @@
         <v>90</v>
       </c>
       <c r="I28" s="5">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="J28" s="5">
         <v>60</v>
@@ -1388,7 +1390,7 @@
         <v>41</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C29" s="5">
         <v>2000</v>

</xml_diff>

<commit_message>
[Feat] (Client) Upload Bin File Also
</commit_message>
<xml_diff>
--- a/CharacterStats.xlsx
+++ b/CharacterStats.xlsx
@@ -72,31 +72,31 @@
     <t>Normal</t>
   </si>
   <si>
+    <t>Chicken</t>
+  </si>
+  <si>
     <t>YellowBird</t>
   </si>
   <si>
-    <t>Chicken</t>
+    <t>Frog</t>
   </si>
   <si>
     <t>MushRoom</t>
   </si>
   <si>
-    <t>Frog</t>
+    <t>Kabu</t>
   </si>
   <si>
     <t>PurpleBeatle</t>
   </si>
   <si>
-    <t>Kabu</t>
+    <t>NormalBear</t>
   </si>
   <si>
     <t>BossDyna</t>
   </si>
   <si>
     <t>Boss</t>
-  </si>
-  <si>
-    <t>NormalBear</t>
   </si>
   <si>
     <t>Scary</t>
@@ -852,13 +852,13 @@
         <v>100</v>
       </c>
       <c r="G14" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H14" s="5">
         <v>50</v>
       </c>
       <c r="I14" s="5">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="J14" s="5">
         <v>0</v>
@@ -887,13 +887,13 @@
         <v>100</v>
       </c>
       <c r="G15" s="5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H15" s="5">
         <v>50</v>
       </c>
       <c r="I15" s="5">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="J15" s="5">
         <v>0</v>
@@ -907,73 +907,73 @@
         <v>25</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="C16" s="5">
-        <v>3000</v>
+        <v>200</v>
       </c>
       <c r="D16" s="5">
-        <v>650</v>
+        <v>40</v>
       </c>
       <c r="E16" s="5">
-        <v>1400</v>
+        <v>500</v>
       </c>
       <c r="F16" s="5">
-        <v>100</v>
+        <v>120</v>
       </c>
       <c r="G16" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H16" s="5">
-        <v>10</v>
+        <v>80</v>
       </c>
       <c r="I16" s="5">
-        <v>350</v>
+        <v>160</v>
       </c>
       <c r="J16" s="5">
         <v>0</v>
       </c>
-      <c r="K16" s="5">
-        <v>400</v>
-      </c>
-      <c r="L16" s="5">
-        <v>650</v>
-      </c>
+      <c r="K16" s="5"/>
+      <c r="L16" s="5"/>
       <c r="M16" s="5"/>
     </row>
     <row r="17" ht="28" customHeight="true" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B17" s="5" t="s">
-        <v>18</v>
-      </c>
       <c r="C17" s="5">
-        <v>200</v>
+        <v>3000</v>
       </c>
       <c r="D17" s="5">
-        <v>40</v>
+        <v>650</v>
       </c>
       <c r="E17" s="5">
-        <v>500</v>
+        <v>1400</v>
       </c>
       <c r="F17" s="5">
-        <v>120</v>
+        <v>100</v>
       </c>
       <c r="G17" s="5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H17" s="5">
-        <v>80</v>
+        <v>10</v>
       </c>
       <c r="I17" s="5">
-        <v>160</v>
+        <v>350</v>
       </c>
       <c r="J17" s="5">
         <v>0</v>
       </c>
-      <c r="K17" s="5"/>
-      <c r="L17" s="5"/>
+      <c r="K17" s="5">
+        <v>400</v>
+      </c>
+      <c r="L17" s="5">
+        <v>650</v>
+      </c>
       <c r="M17" s="5"/>
     </row>
     <row r="18" ht="28" customHeight="true" x14ac:dyDescent="0.25">
@@ -1160,7 +1160,7 @@
         <v>35</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C23" s="5">
         <v>300</v>
@@ -1273,7 +1273,7 @@
         <v>38</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C26" s="5">
         <v>2500</v>
@@ -1312,7 +1312,7 @@
         <v>39</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C27" s="5">
         <v>2500</v>
@@ -1351,7 +1351,7 @@
         <v>40</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C28" s="5">
         <v>1500</v>
@@ -1390,7 +1390,7 @@
         <v>41</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C29" s="5">
         <v>2000</v>

</xml_diff>

<commit_message>
[Feat] (Client) Fixed Wrong Data Insert From Excel
</commit_message>
<xml_diff>
--- a/CharacterStats.xlsx
+++ b/CharacterStats.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="63" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="65" uniqueCount="43">
   <si>
     <t>Created by LibXL trial version 4.0.3. Please buy the LibXL full version for removing this message.</t>
   </si>
@@ -72,33 +72,33 @@
     <t>Normal</t>
   </si>
   <si>
+    <t>YellowBird</t>
+  </si>
+  <si>
     <t>Chicken</t>
   </si>
   <si>
-    <t>YellowBird</t>
+    <t>MushRoom</t>
   </si>
   <si>
     <t>Frog</t>
   </si>
   <si>
-    <t>MushRoom</t>
+    <t>PurpleBeatle</t>
   </si>
   <si>
     <t>Kabu</t>
   </si>
   <si>
-    <t>PurpleBeatle</t>
+    <t>BossDyna</t>
+  </si>
+  <si>
+    <t>Boss</t>
   </si>
   <si>
     <t>NormalBear</t>
   </si>
   <si>
-    <t>BossDyna</t>
-  </si>
-  <si>
-    <t>Boss</t>
-  </si>
-  <si>
     <t>Scary</t>
   </si>
   <si>
@@ -121,6 +121,9 @@
   </si>
   <si>
     <t>Fight</t>
+  </si>
+  <si>
+    <t>Buy me !</t>
   </si>
   <si>
     <t>Fire</t>
@@ -852,13 +855,13 @@
         <v>100</v>
       </c>
       <c r="G14" s="5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H14" s="5">
         <v>50</v>
       </c>
       <c r="I14" s="5">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="J14" s="5">
         <v>0</v>
@@ -887,13 +890,13 @@
         <v>100</v>
       </c>
       <c r="G15" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H15" s="5">
         <v>50</v>
       </c>
       <c r="I15" s="5">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="J15" s="5">
         <v>0</v>
@@ -907,73 +910,73 @@
         <v>25</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="C16" s="5">
-        <v>200</v>
+        <v>3000</v>
       </c>
       <c r="D16" s="5">
-        <v>40</v>
+        <v>650</v>
       </c>
       <c r="E16" s="5">
-        <v>500</v>
+        <v>1400</v>
       </c>
       <c r="F16" s="5">
-        <v>120</v>
+        <v>100</v>
       </c>
       <c r="G16" s="5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H16" s="5">
-        <v>80</v>
+        <v>10</v>
       </c>
       <c r="I16" s="5">
-        <v>160</v>
+        <v>350</v>
       </c>
       <c r="J16" s="5">
         <v>0</v>
       </c>
-      <c r="K16" s="5"/>
-      <c r="L16" s="5"/>
+      <c r="K16" s="5">
+        <v>400</v>
+      </c>
+      <c r="L16" s="5">
+        <v>650</v>
+      </c>
       <c r="M16" s="5"/>
     </row>
     <row r="17" ht="28" customHeight="true" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="C17" s="5">
-        <v>3000</v>
+        <v>200</v>
       </c>
       <c r="D17" s="5">
-        <v>650</v>
+        <v>40</v>
       </c>
       <c r="E17" s="5">
-        <v>1400</v>
+        <v>500</v>
       </c>
       <c r="F17" s="5">
-        <v>100</v>
+        <v>120</v>
       </c>
       <c r="G17" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H17" s="5">
-        <v>10</v>
+        <v>80</v>
       </c>
       <c r="I17" s="5">
-        <v>350</v>
+        <v>160</v>
       </c>
       <c r="J17" s="5">
         <v>0</v>
       </c>
-      <c r="K17" s="5">
-        <v>400</v>
-      </c>
-      <c r="L17" s="5">
-        <v>650</v>
-      </c>
+      <c r="K17" s="5"/>
+      <c r="L17" s="5"/>
       <c r="M17" s="5"/>
     </row>
     <row r="18" ht="28" customHeight="true" x14ac:dyDescent="0.25">
@@ -1160,7 +1163,7 @@
         <v>35</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="C23" s="5">
         <v>300</v>
@@ -1180,23 +1183,21 @@
       <c r="H23" s="5">
         <v>90</v>
       </c>
-      <c r="I23" s="5">
-        <v>100</v>
+      <c r="I23" s="5" t="s">
+        <v>36</v>
       </c>
       <c r="J23" s="5">
         <v>0</v>
       </c>
-      <c r="K23" s="5">
-        <v>0</v>
-      </c>
-      <c r="L23" s="5">
-        <v>0</v>
-      </c>
-      <c r="M23" s="5"/>
+      <c r="K23" s="5"/>
+      <c r="L23" s="5"/>
+      <c r="M23" s="5" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="24" ht="28" customHeight="true" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>33</v>
@@ -1228,12 +1229,12 @@
       <c r="K24" s="5"/>
       <c r="L24" s="5"/>
       <c r="M24" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="25" ht="28" customHeight="true" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B25" s="5" t="s">
         <v>33</v>
@@ -1265,15 +1266,15 @@
       <c r="K25" s="5"/>
       <c r="L25" s="5"/>
       <c r="M25" s="5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="26" ht="28" customHeight="true" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C26" s="5">
         <v>2500</v>
@@ -1309,10 +1310,10 @@
     </row>
     <row r="27" ht="28" customHeight="true" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C27" s="5">
         <v>2500</v>
@@ -1348,10 +1349,10 @@
     </row>
     <row r="28" ht="28" customHeight="true" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C28" s="5">
         <v>1500</v>
@@ -1363,7 +1364,7 @@
         <v>1000</v>
       </c>
       <c r="F28" s="5">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="G28" s="5" t="b">
         <v>1</v>
@@ -1372,7 +1373,7 @@
         <v>90</v>
       </c>
       <c r="I28" s="5">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="J28" s="5">
         <v>60</v>
@@ -1387,10 +1388,10 @@
     </row>
     <row r="29" ht="28" customHeight="true" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C29" s="5">
         <v>2000</v>

</xml_diff>

<commit_message>
[Feat] (Client) Linked libxl.lib File To Project Also In Release Mode
</commit_message>
<xml_diff>
--- a/CharacterStats.xlsx
+++ b/CharacterStats.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="65" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="64" uniqueCount="42">
   <si>
     <t>Created by LibXL trial version 4.0.3. Please buy the LibXL full version for removing this message.</t>
   </si>
@@ -72,22 +72,25 @@
     <t>Normal</t>
   </si>
   <si>
+    <t>Chicken</t>
+  </si>
+  <si>
     <t>YellowBird</t>
   </si>
   <si>
-    <t>Chicken</t>
+    <t>Frog</t>
   </si>
   <si>
     <t>MushRoom</t>
   </si>
   <si>
-    <t>Frog</t>
+    <t>Kabu</t>
   </si>
   <si>
     <t>PurpleBeatle</t>
   </si>
   <si>
-    <t>Kabu</t>
+    <t>NormalBear</t>
   </si>
   <si>
     <t>BossDyna</t>
@@ -96,9 +99,6 @@
     <t>Boss</t>
   </si>
   <si>
-    <t>NormalBear</t>
-  </si>
-  <si>
     <t>Scary</t>
   </si>
   <si>
@@ -121,9 +121,6 @@
   </si>
   <si>
     <t>Fight</t>
-  </si>
-  <si>
-    <t>Buy me !</t>
   </si>
   <si>
     <t>Fire</t>
@@ -855,13 +852,13 @@
         <v>100</v>
       </c>
       <c r="G14" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H14" s="5">
         <v>50</v>
       </c>
       <c r="I14" s="5">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="J14" s="5">
         <v>0</v>
@@ -890,13 +887,13 @@
         <v>100</v>
       </c>
       <c r="G15" s="5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H15" s="5">
         <v>50</v>
       </c>
       <c r="I15" s="5">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="J15" s="5">
         <v>0</v>
@@ -910,73 +907,73 @@
         <v>25</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="C16" s="5">
-        <v>3000</v>
+        <v>200</v>
       </c>
       <c r="D16" s="5">
-        <v>650</v>
+        <v>40</v>
       </c>
       <c r="E16" s="5">
-        <v>1400</v>
+        <v>500</v>
       </c>
       <c r="F16" s="5">
-        <v>100</v>
+        <v>120</v>
       </c>
       <c r="G16" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H16" s="5">
-        <v>10</v>
+        <v>80</v>
       </c>
       <c r="I16" s="5">
-        <v>350</v>
+        <v>160</v>
       </c>
       <c r="J16" s="5">
         <v>0</v>
       </c>
-      <c r="K16" s="5">
-        <v>400</v>
-      </c>
-      <c r="L16" s="5">
-        <v>650</v>
-      </c>
+      <c r="K16" s="5"/>
+      <c r="L16" s="5"/>
       <c r="M16" s="5"/>
     </row>
     <row r="17" ht="28" customHeight="true" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B17" s="5" t="s">
-        <v>18</v>
-      </c>
       <c r="C17" s="5">
-        <v>200</v>
+        <v>3000</v>
       </c>
       <c r="D17" s="5">
-        <v>40</v>
+        <v>650</v>
       </c>
       <c r="E17" s="5">
-        <v>500</v>
+        <v>1400</v>
       </c>
       <c r="F17" s="5">
-        <v>120</v>
+        <v>100</v>
       </c>
       <c r="G17" s="5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H17" s="5">
-        <v>80</v>
+        <v>10</v>
       </c>
       <c r="I17" s="5">
-        <v>160</v>
+        <v>350</v>
       </c>
       <c r="J17" s="5">
         <v>0</v>
       </c>
-      <c r="K17" s="5"/>
-      <c r="L17" s="5"/>
+      <c r="K17" s="5">
+        <v>400</v>
+      </c>
+      <c r="L17" s="5">
+        <v>650</v>
+      </c>
       <c r="M17" s="5"/>
     </row>
     <row r="18" ht="28" customHeight="true" x14ac:dyDescent="0.25">
@@ -1183,8 +1180,8 @@
       <c r="H23" s="5">
         <v>90</v>
       </c>
-      <c r="I23" s="5" t="s">
-        <v>36</v>
+      <c r="I23" s="5">
+        <v>0</v>
       </c>
       <c r="J23" s="5">
         <v>0</v>
@@ -1197,7 +1194,7 @@
     </row>
     <row r="24" ht="28" customHeight="true" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>33</v>
@@ -1229,12 +1226,12 @@
       <c r="K24" s="5"/>
       <c r="L24" s="5"/>
       <c r="M24" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="25" ht="28" customHeight="true" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B25" s="5" t="s">
         <v>33</v>
@@ -1266,15 +1263,15 @@
       <c r="K25" s="5"/>
       <c r="L25" s="5"/>
       <c r="M25" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="26" ht="28" customHeight="true" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C26" s="5">
         <v>2500</v>
@@ -1310,10 +1307,10 @@
     </row>
     <row r="27" ht="28" customHeight="true" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C27" s="5">
         <v>2500</v>
@@ -1349,10 +1346,10 @@
     </row>
     <row r="28" ht="28" customHeight="true" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C28" s="5">
         <v>1500</v>
@@ -1388,10 +1385,10 @@
     </row>
     <row r="29" ht="28" customHeight="true" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C29" s="5">
         <v>2000</v>

</xml_diff>

<commit_message>
[Feat] (Client) Do Not Show Collider Color In ReleaseMode
</commit_message>
<xml_diff>
--- a/CharacterStats.xlsx
+++ b/CharacterStats.xlsx
@@ -72,31 +72,31 @@
     <t>Normal</t>
   </si>
   <si>
+    <t>YellowBird</t>
+  </si>
+  <si>
     <t>Chicken</t>
   </si>
   <si>
-    <t>YellowBird</t>
+    <t>MushRoom</t>
   </si>
   <si>
     <t>Frog</t>
   </si>
   <si>
-    <t>MushRoom</t>
+    <t>PurpleBeatle</t>
   </si>
   <si>
     <t>Kabu</t>
   </si>
   <si>
-    <t>PurpleBeatle</t>
+    <t>BossDyna</t>
+  </si>
+  <si>
+    <t>Boss</t>
   </si>
   <si>
     <t>NormalBear</t>
-  </si>
-  <si>
-    <t>BossDyna</t>
-  </si>
-  <si>
-    <t>Boss</t>
   </si>
   <si>
     <t>Scary</t>
@@ -852,13 +852,13 @@
         <v>100</v>
       </c>
       <c r="G14" s="5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H14" s="5">
         <v>50</v>
       </c>
       <c r="I14" s="5">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="J14" s="5">
         <v>0</v>
@@ -887,13 +887,13 @@
         <v>100</v>
       </c>
       <c r="G15" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H15" s="5">
         <v>50</v>
       </c>
       <c r="I15" s="5">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="J15" s="5">
         <v>0</v>
@@ -907,73 +907,73 @@
         <v>25</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="C16" s="5">
-        <v>200</v>
+        <v>3000</v>
       </c>
       <c r="D16" s="5">
-        <v>40</v>
+        <v>650</v>
       </c>
       <c r="E16" s="5">
-        <v>500</v>
+        <v>1400</v>
       </c>
       <c r="F16" s="5">
-        <v>120</v>
+        <v>100</v>
       </c>
       <c r="G16" s="5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H16" s="5">
-        <v>80</v>
+        <v>10</v>
       </c>
       <c r="I16" s="5">
-        <v>160</v>
+        <v>350</v>
       </c>
       <c r="J16" s="5">
         <v>0</v>
       </c>
-      <c r="K16" s="5"/>
-      <c r="L16" s="5"/>
+      <c r="K16" s="5">
+        <v>400</v>
+      </c>
+      <c r="L16" s="5">
+        <v>650</v>
+      </c>
       <c r="M16" s="5"/>
     </row>
     <row r="17" ht="28" customHeight="true" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="C17" s="5">
-        <v>3000</v>
+        <v>200</v>
       </c>
       <c r="D17" s="5">
-        <v>650</v>
+        <v>40</v>
       </c>
       <c r="E17" s="5">
-        <v>1400</v>
+        <v>500</v>
       </c>
       <c r="F17" s="5">
-        <v>100</v>
+        <v>120</v>
       </c>
       <c r="G17" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H17" s="5">
-        <v>10</v>
+        <v>80</v>
       </c>
       <c r="I17" s="5">
-        <v>350</v>
+        <v>160</v>
       </c>
       <c r="J17" s="5">
         <v>0</v>
       </c>
-      <c r="K17" s="5">
-        <v>400</v>
-      </c>
-      <c r="L17" s="5">
-        <v>650</v>
-      </c>
+      <c r="K17" s="5"/>
+      <c r="L17" s="5"/>
       <c r="M17" s="5"/>
     </row>
     <row r="18" ht="28" customHeight="true" x14ac:dyDescent="0.25">
@@ -1271,7 +1271,7 @@
         <v>38</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C26" s="5">
         <v>2500</v>
@@ -1310,7 +1310,7 @@
         <v>39</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C27" s="5">
         <v>2500</v>
@@ -1349,7 +1349,7 @@
         <v>40</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C28" s="5">
         <v>1500</v>
@@ -1388,7 +1388,7 @@
         <v>41</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C29" s="5">
         <v>2000</v>

</xml_diff>

<commit_message>
[Fix] (Client) Set Line Start, EndBos Opacity As 0.f In ReleaseMode
</commit_message>
<xml_diff>
--- a/CharacterStats.xlsx
+++ b/CharacterStats.xlsx
@@ -72,31 +72,31 @@
     <t>Normal</t>
   </si>
   <si>
+    <t>Chicken</t>
+  </si>
+  <si>
     <t>YellowBird</t>
   </si>
   <si>
-    <t>Chicken</t>
+    <t>Frog</t>
   </si>
   <si>
     <t>MushRoom</t>
   </si>
   <si>
-    <t>Frog</t>
+    <t>Kabu</t>
   </si>
   <si>
     <t>PurpleBeatle</t>
   </si>
   <si>
-    <t>Kabu</t>
+    <t>NormalBear</t>
   </si>
   <si>
     <t>BossDyna</t>
   </si>
   <si>
     <t>Boss</t>
-  </si>
-  <si>
-    <t>NormalBear</t>
   </si>
   <si>
     <t>Scary</t>
@@ -852,13 +852,13 @@
         <v>100</v>
       </c>
       <c r="G14" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H14" s="5">
         <v>50</v>
       </c>
       <c r="I14" s="5">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="J14" s="5">
         <v>0</v>
@@ -887,13 +887,13 @@
         <v>100</v>
       </c>
       <c r="G15" s="5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H15" s="5">
         <v>50</v>
       </c>
       <c r="I15" s="5">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="J15" s="5">
         <v>0</v>
@@ -907,73 +907,73 @@
         <v>25</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="C16" s="5">
-        <v>3000</v>
+        <v>200</v>
       </c>
       <c r="D16" s="5">
-        <v>650</v>
+        <v>40</v>
       </c>
       <c r="E16" s="5">
-        <v>1400</v>
+        <v>500</v>
       </c>
       <c r="F16" s="5">
-        <v>100</v>
+        <v>120</v>
       </c>
       <c r="G16" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H16" s="5">
-        <v>10</v>
+        <v>80</v>
       </c>
       <c r="I16" s="5">
-        <v>350</v>
+        <v>160</v>
       </c>
       <c r="J16" s="5">
         <v>0</v>
       </c>
-      <c r="K16" s="5">
-        <v>400</v>
-      </c>
-      <c r="L16" s="5">
-        <v>650</v>
-      </c>
+      <c r="K16" s="5"/>
+      <c r="L16" s="5"/>
       <c r="M16" s="5"/>
     </row>
     <row r="17" ht="28" customHeight="true" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B17" s="5" t="s">
-        <v>18</v>
-      </c>
       <c r="C17" s="5">
-        <v>200</v>
+        <v>3000</v>
       </c>
       <c r="D17" s="5">
-        <v>40</v>
+        <v>650</v>
       </c>
       <c r="E17" s="5">
-        <v>500</v>
+        <v>1400</v>
       </c>
       <c r="F17" s="5">
-        <v>120</v>
+        <v>100</v>
       </c>
       <c r="G17" s="5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H17" s="5">
-        <v>80</v>
+        <v>10</v>
       </c>
       <c r="I17" s="5">
-        <v>160</v>
+        <v>350</v>
       </c>
       <c r="J17" s="5">
         <v>0</v>
       </c>
-      <c r="K17" s="5"/>
-      <c r="L17" s="5"/>
+      <c r="K17" s="5">
+        <v>400</v>
+      </c>
+      <c r="L17" s="5">
+        <v>650</v>
+      </c>
       <c r="M17" s="5"/>
     </row>
     <row r="18" ht="28" customHeight="true" x14ac:dyDescent="0.25">
@@ -1271,7 +1271,7 @@
         <v>38</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C26" s="5">
         <v>2500</v>
@@ -1310,7 +1310,7 @@
         <v>39</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C27" s="5">
         <v>2500</v>
@@ -1349,7 +1349,7 @@
         <v>40</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C28" s="5">
         <v>1500</v>
@@ -1388,7 +1388,7 @@
         <v>41</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C29" s="5">
         <v>2000</v>

</xml_diff>

<commit_message>
[Feat] (Client) Prevent Player Animation Not Being UpAttack Animation While GoUp Attacking In Fire, Sword Kirby
</commit_message>
<xml_diff>
--- a/CharacterStats.xlsx
+++ b/CharacterStats.xlsx
@@ -72,31 +72,31 @@
     <t>Normal</t>
   </si>
   <si>
+    <t>YellowBird</t>
+  </si>
+  <si>
     <t>Chicken</t>
   </si>
   <si>
-    <t>YellowBird</t>
+    <t>MushRoom</t>
   </si>
   <si>
     <t>Frog</t>
   </si>
   <si>
-    <t>MushRoom</t>
+    <t>PurpleBeatle</t>
   </si>
   <si>
     <t>Kabu</t>
   </si>
   <si>
-    <t>PurpleBeatle</t>
+    <t>BossDyna</t>
+  </si>
+  <si>
+    <t>Boss</t>
   </si>
   <si>
     <t>NormalBear</t>
-  </si>
-  <si>
-    <t>BossDyna</t>
-  </si>
-  <si>
-    <t>Boss</t>
   </si>
   <si>
     <t>Scary</t>
@@ -852,13 +852,13 @@
         <v>100</v>
       </c>
       <c r="G14" s="5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H14" s="5">
         <v>50</v>
       </c>
       <c r="I14" s="5">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="J14" s="5">
         <v>0</v>
@@ -887,13 +887,13 @@
         <v>100</v>
       </c>
       <c r="G15" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H15" s="5">
         <v>50</v>
       </c>
       <c r="I15" s="5">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="J15" s="5">
         <v>0</v>
@@ -907,73 +907,73 @@
         <v>25</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="C16" s="5">
-        <v>200</v>
+        <v>3000</v>
       </c>
       <c r="D16" s="5">
-        <v>40</v>
+        <v>650</v>
       </c>
       <c r="E16" s="5">
-        <v>500</v>
+        <v>1400</v>
       </c>
       <c r="F16" s="5">
-        <v>120</v>
+        <v>100</v>
       </c>
       <c r="G16" s="5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H16" s="5">
-        <v>80</v>
+        <v>10</v>
       </c>
       <c r="I16" s="5">
-        <v>160</v>
+        <v>350</v>
       </c>
       <c r="J16" s="5">
         <v>0</v>
       </c>
-      <c r="K16" s="5"/>
-      <c r="L16" s="5"/>
+      <c r="K16" s="5">
+        <v>400</v>
+      </c>
+      <c r="L16" s="5">
+        <v>650</v>
+      </c>
       <c r="M16" s="5"/>
     </row>
     <row r="17" ht="28" customHeight="true" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="C17" s="5">
-        <v>3000</v>
+        <v>200</v>
       </c>
       <c r="D17" s="5">
-        <v>650</v>
+        <v>40</v>
       </c>
       <c r="E17" s="5">
-        <v>1400</v>
+        <v>500</v>
       </c>
       <c r="F17" s="5">
-        <v>100</v>
+        <v>120</v>
       </c>
       <c r="G17" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H17" s="5">
-        <v>10</v>
+        <v>80</v>
       </c>
       <c r="I17" s="5">
-        <v>350</v>
+        <v>160</v>
       </c>
       <c r="J17" s="5">
         <v>0</v>
       </c>
-      <c r="K17" s="5">
-        <v>400</v>
-      </c>
-      <c r="L17" s="5">
-        <v>650</v>
-      </c>
+      <c r="K17" s="5"/>
+      <c r="L17" s="5"/>
       <c r="M17" s="5"/>
     </row>
     <row r="18" ht="28" customHeight="true" x14ac:dyDescent="0.25">
@@ -1271,7 +1271,7 @@
         <v>38</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C26" s="5">
         <v>2500</v>
@@ -1310,7 +1310,7 @@
         <v>39</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C27" s="5">
         <v>2500</v>
@@ -1349,7 +1349,7 @@
         <v>40</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C28" s="5">
         <v>1500</v>
@@ -1388,7 +1388,7 @@
         <v>41</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C29" s="5">
         <v>2000</v>

</xml_diff>

<commit_message>
[Feat] (Client) Beam Kirby Ultimate Attack Make Usage Of KirbyAttackObjectPool
</commit_message>
<xml_diff>
--- a/CharacterStats.xlsx
+++ b/CharacterStats.xlsx
@@ -910,10 +910,10 @@
         <v>26</v>
       </c>
       <c r="C16" s="5">
-        <v>3000</v>
+        <v>2500</v>
       </c>
       <c r="D16" s="5">
-        <v>650</v>
+        <v>1005</v>
       </c>
       <c r="E16" s="5">
         <v>1400</v>
@@ -925,7 +925,7 @@
         <v>0</v>
       </c>
       <c r="H16" s="5">
-        <v>10</v>
+        <v>90</v>
       </c>
       <c r="I16" s="5">
         <v>350</v>
@@ -934,10 +934,10 @@
         <v>0</v>
       </c>
       <c r="K16" s="5">
-        <v>400</v>
+        <v>600</v>
       </c>
       <c r="L16" s="5">
-        <v>650</v>
+        <v>1000</v>
       </c>
       <c r="M16" s="5"/>
     </row>
@@ -958,7 +958,7 @@
         <v>500</v>
       </c>
       <c r="F17" s="5">
-        <v>120</v>
+        <v>150</v>
       </c>
       <c r="G17" s="5" t="b">
         <v>1</v>
@@ -1141,7 +1141,7 @@
         <v>1</v>
       </c>
       <c r="H22" s="5">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="I22" s="5">
         <v>100</v>
@@ -1361,7 +1361,7 @@
         <v>1000</v>
       </c>
       <c r="F28" s="5">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="G28" s="5" t="b">
         <v>1</v>

</xml_diff>

<commit_message>
[Feat] (Client) Fight Kirby Use KirbyAttack Object Pool When It Ultimate Attacks
</commit_message>
<xml_diff>
--- a/CharacterStats.xlsx
+++ b/CharacterStats.xlsx
@@ -72,31 +72,31 @@
     <t>Normal</t>
   </si>
   <si>
+    <t>Chicken</t>
+  </si>
+  <si>
     <t>YellowBird</t>
   </si>
   <si>
-    <t>Chicken</t>
+    <t>Frog</t>
   </si>
   <si>
     <t>MushRoom</t>
   </si>
   <si>
-    <t>Frog</t>
+    <t>Kabu</t>
   </si>
   <si>
     <t>PurpleBeatle</t>
   </si>
   <si>
-    <t>Kabu</t>
+    <t>NormalBear</t>
   </si>
   <si>
     <t>BossDyna</t>
   </si>
   <si>
     <t>Boss</t>
-  </si>
-  <si>
-    <t>NormalBear</t>
   </si>
   <si>
     <t>Scary</t>
@@ -852,13 +852,13 @@
         <v>100</v>
       </c>
       <c r="G14" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H14" s="5">
         <v>50</v>
       </c>
       <c r="I14" s="5">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="J14" s="5">
         <v>0</v>
@@ -887,13 +887,13 @@
         <v>100</v>
       </c>
       <c r="G15" s="5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H15" s="5">
         <v>50</v>
       </c>
       <c r="I15" s="5">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="J15" s="5">
         <v>0</v>
@@ -907,73 +907,73 @@
         <v>25</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="C16" s="5">
-        <v>2500</v>
+        <v>200</v>
       </c>
       <c r="D16" s="5">
-        <v>1005</v>
+        <v>40</v>
       </c>
       <c r="E16" s="5">
-        <v>1400</v>
+        <v>500</v>
       </c>
       <c r="F16" s="5">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="G16" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H16" s="5">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="I16" s="5">
-        <v>350</v>
+        <v>160</v>
       </c>
       <c r="J16" s="5">
         <v>0</v>
       </c>
-      <c r="K16" s="5">
-        <v>600</v>
-      </c>
-      <c r="L16" s="5">
-        <v>1000</v>
-      </c>
+      <c r="K16" s="5"/>
+      <c r="L16" s="5"/>
       <c r="M16" s="5"/>
     </row>
     <row r="17" ht="28" customHeight="true" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B17" s="5" t="s">
-        <v>18</v>
-      </c>
       <c r="C17" s="5">
-        <v>200</v>
+        <v>2500</v>
       </c>
       <c r="D17" s="5">
-        <v>40</v>
+        <v>1005</v>
       </c>
       <c r="E17" s="5">
-        <v>500</v>
+        <v>1400</v>
       </c>
       <c r="F17" s="5">
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="G17" s="5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H17" s="5">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="I17" s="5">
-        <v>160</v>
+        <v>350</v>
       </c>
       <c r="J17" s="5">
         <v>0</v>
       </c>
-      <c r="K17" s="5"/>
-      <c r="L17" s="5"/>
+      <c r="K17" s="5">
+        <v>600</v>
+      </c>
+      <c r="L17" s="5">
+        <v>1000</v>
+      </c>
       <c r="M17" s="5"/>
     </row>
     <row r="18" ht="28" customHeight="true" x14ac:dyDescent="0.25">
@@ -1271,7 +1271,7 @@
         <v>38</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C26" s="5">
         <v>2500</v>
@@ -1310,7 +1310,7 @@
         <v>39</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C27" s="5">
         <v>2500</v>
@@ -1349,7 +1349,7 @@
         <v>40</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C28" s="5">
         <v>1500</v>
@@ -1388,7 +1388,7 @@
         <v>41</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C29" s="5">
         <v>2000</v>

</xml_diff>

<commit_message>
[Feat] (Client) Fight Kirby Ultimate Attack Effect Pos Set In Random Pos Properly
</commit_message>
<xml_diff>
--- a/CharacterStats.xlsx
+++ b/CharacterStats.xlsx
@@ -72,31 +72,31 @@
     <t>Normal</t>
   </si>
   <si>
+    <t>YellowBird</t>
+  </si>
+  <si>
     <t>Chicken</t>
   </si>
   <si>
-    <t>YellowBird</t>
+    <t>MushRoom</t>
   </si>
   <si>
     <t>Frog</t>
   </si>
   <si>
-    <t>MushRoom</t>
+    <t>PurpleBeatle</t>
   </si>
   <si>
     <t>Kabu</t>
   </si>
   <si>
-    <t>PurpleBeatle</t>
+    <t>BossDyna</t>
+  </si>
+  <si>
+    <t>Boss</t>
   </si>
   <si>
     <t>NormalBear</t>
-  </si>
-  <si>
-    <t>BossDyna</t>
-  </si>
-  <si>
-    <t>Boss</t>
   </si>
   <si>
     <t>Scary</t>
@@ -852,13 +852,13 @@
         <v>100</v>
       </c>
       <c r="G14" s="5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H14" s="5">
         <v>50</v>
       </c>
       <c r="I14" s="5">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="J14" s="5">
         <v>0</v>
@@ -887,13 +887,13 @@
         <v>100</v>
       </c>
       <c r="G15" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H15" s="5">
         <v>50</v>
       </c>
       <c r="I15" s="5">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="J15" s="5">
         <v>0</v>
@@ -907,73 +907,73 @@
         <v>25</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="C16" s="5">
-        <v>200</v>
+        <v>2500</v>
       </c>
       <c r="D16" s="5">
-        <v>40</v>
+        <v>1005</v>
       </c>
       <c r="E16" s="5">
-        <v>500</v>
+        <v>1400</v>
       </c>
       <c r="F16" s="5">
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="G16" s="5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H16" s="5">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="I16" s="5">
-        <v>160</v>
+        <v>350</v>
       </c>
       <c r="J16" s="5">
         <v>0</v>
       </c>
-      <c r="K16" s="5"/>
-      <c r="L16" s="5"/>
+      <c r="K16" s="5">
+        <v>600</v>
+      </c>
+      <c r="L16" s="5">
+        <v>1000</v>
+      </c>
       <c r="M16" s="5"/>
     </row>
     <row r="17" ht="28" customHeight="true" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="C17" s="5">
-        <v>2500</v>
+        <v>200</v>
       </c>
       <c r="D17" s="5">
-        <v>1005</v>
+        <v>40</v>
       </c>
       <c r="E17" s="5">
-        <v>1400</v>
+        <v>500</v>
       </c>
       <c r="F17" s="5">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="G17" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H17" s="5">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="I17" s="5">
-        <v>350</v>
+        <v>160</v>
       </c>
       <c r="J17" s="5">
         <v>0</v>
       </c>
-      <c r="K17" s="5">
-        <v>600</v>
-      </c>
-      <c r="L17" s="5">
-        <v>1000</v>
-      </c>
+      <c r="K17" s="5"/>
+      <c r="L17" s="5"/>
       <c r="M17" s="5"/>
     </row>
     <row r="18" ht="28" customHeight="true" x14ac:dyDescent="0.25">
@@ -1271,13 +1271,13 @@
         <v>38</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C26" s="5">
         <v>2500</v>
       </c>
       <c r="D26" s="5">
-        <v>600</v>
+        <v>0</v>
       </c>
       <c r="E26" s="5">
         <v>1200</v>
@@ -1310,7 +1310,7 @@
         <v>39</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C27" s="5">
         <v>2500</v>
@@ -1349,7 +1349,7 @@
         <v>40</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C28" s="5">
         <v>1500</v>
@@ -1388,7 +1388,7 @@
         <v>41</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C29" s="5">
         <v>2000</v>

</xml_diff>

<commit_message>
[Feat] (Client) Beam Kirby Ultimate Attack Effect Pos Set In Random Pos Properly
</commit_message>
<xml_diff>
--- a/CharacterStats.xlsx
+++ b/CharacterStats.xlsx
@@ -72,31 +72,31 @@
     <t>Normal</t>
   </si>
   <si>
+    <t>Chicken</t>
+  </si>
+  <si>
     <t>YellowBird</t>
   </si>
   <si>
-    <t>Chicken</t>
+    <t>Frog</t>
   </si>
   <si>
     <t>MushRoom</t>
   </si>
   <si>
-    <t>Frog</t>
+    <t>Kabu</t>
   </si>
   <si>
     <t>PurpleBeatle</t>
   </si>
   <si>
-    <t>Kabu</t>
+    <t>NormalBear</t>
   </si>
   <si>
     <t>BossDyna</t>
   </si>
   <si>
     <t>Boss</t>
-  </si>
-  <si>
-    <t>NormalBear</t>
   </si>
   <si>
     <t>Scary</t>
@@ -852,13 +852,13 @@
         <v>100</v>
       </c>
       <c r="G14" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H14" s="5">
         <v>50</v>
       </c>
       <c r="I14" s="5">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="J14" s="5">
         <v>0</v>
@@ -887,13 +887,13 @@
         <v>100</v>
       </c>
       <c r="G15" s="5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H15" s="5">
         <v>50</v>
       </c>
       <c r="I15" s="5">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="J15" s="5">
         <v>0</v>
@@ -907,73 +907,73 @@
         <v>25</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="C16" s="5">
-        <v>2500</v>
+        <v>200</v>
       </c>
       <c r="D16" s="5">
-        <v>1005</v>
+        <v>40</v>
       </c>
       <c r="E16" s="5">
-        <v>1400</v>
+        <v>500</v>
       </c>
       <c r="F16" s="5">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="G16" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H16" s="5">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="I16" s="5">
-        <v>350</v>
+        <v>160</v>
       </c>
       <c r="J16" s="5">
         <v>0</v>
       </c>
-      <c r="K16" s="5">
-        <v>600</v>
-      </c>
-      <c r="L16" s="5">
-        <v>1000</v>
-      </c>
+      <c r="K16" s="5"/>
+      <c r="L16" s="5"/>
       <c r="M16" s="5"/>
     </row>
     <row r="17" ht="28" customHeight="true" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B17" s="5" t="s">
-        <v>18</v>
-      </c>
       <c r="C17" s="5">
-        <v>200</v>
+        <v>2500</v>
       </c>
       <c r="D17" s="5">
-        <v>40</v>
+        <v>1005</v>
       </c>
       <c r="E17" s="5">
-        <v>500</v>
+        <v>1400</v>
       </c>
       <c r="F17" s="5">
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="G17" s="5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H17" s="5">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="I17" s="5">
-        <v>160</v>
+        <v>350</v>
       </c>
       <c r="J17" s="5">
         <v>0</v>
       </c>
-      <c r="K17" s="5"/>
-      <c r="L17" s="5"/>
+      <c r="K17" s="5">
+        <v>600</v>
+      </c>
+      <c r="L17" s="5">
+        <v>1000</v>
+      </c>
       <c r="M17" s="5"/>
     </row>
     <row r="18" ht="28" customHeight="true" x14ac:dyDescent="0.25">
@@ -1271,7 +1271,7 @@
         <v>38</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C26" s="5">
         <v>2500</v>
@@ -1310,7 +1310,7 @@
         <v>39</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C27" s="5">
         <v>2500</v>
@@ -1349,7 +1349,7 @@
         <v>40</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C28" s="5">
         <v>1500</v>
@@ -1388,7 +1388,7 @@
         <v>41</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C29" s="5">
         <v>2000</v>

</xml_diff>

<commit_message>
[Feat] (Engine) Create Gaussian Sample Function In Shader Which Extract Random R Value From Texture
</commit_message>
<xml_diff>
--- a/CharacterStats.xlsx
+++ b/CharacterStats.xlsx
@@ -72,31 +72,31 @@
     <t>Normal</t>
   </si>
   <si>
+    <t>YellowBird</t>
+  </si>
+  <si>
     <t>Chicken</t>
   </si>
   <si>
-    <t>YellowBird</t>
+    <t>MushRoom</t>
   </si>
   <si>
     <t>Frog</t>
   </si>
   <si>
-    <t>MushRoom</t>
+    <t>PurpleBeatle</t>
   </si>
   <si>
     <t>Kabu</t>
   </si>
   <si>
-    <t>PurpleBeatle</t>
+    <t>BossDyna</t>
+  </si>
+  <si>
+    <t>Boss</t>
   </si>
   <si>
     <t>NormalBear</t>
-  </si>
-  <si>
-    <t>BossDyna</t>
-  </si>
-  <si>
-    <t>Boss</t>
   </si>
   <si>
     <t>Scary</t>
@@ -852,13 +852,13 @@
         <v>100</v>
       </c>
       <c r="G14" s="5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H14" s="5">
         <v>50</v>
       </c>
       <c r="I14" s="5">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="J14" s="5">
         <v>0</v>
@@ -887,13 +887,13 @@
         <v>100</v>
       </c>
       <c r="G15" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H15" s="5">
         <v>50</v>
       </c>
       <c r="I15" s="5">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="J15" s="5">
         <v>0</v>
@@ -907,73 +907,73 @@
         <v>25</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="C16" s="5">
-        <v>200</v>
+        <v>2500</v>
       </c>
       <c r="D16" s="5">
-        <v>40</v>
+        <v>1005</v>
       </c>
       <c r="E16" s="5">
-        <v>500</v>
+        <v>1400</v>
       </c>
       <c r="F16" s="5">
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="G16" s="5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H16" s="5">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="I16" s="5">
-        <v>160</v>
+        <v>350</v>
       </c>
       <c r="J16" s="5">
         <v>0</v>
       </c>
-      <c r="K16" s="5"/>
-      <c r="L16" s="5"/>
+      <c r="K16" s="5">
+        <v>600</v>
+      </c>
+      <c r="L16" s="5">
+        <v>1000</v>
+      </c>
       <c r="M16" s="5"/>
     </row>
     <row r="17" ht="28" customHeight="true" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="C17" s="5">
-        <v>2500</v>
+        <v>200</v>
       </c>
       <c r="D17" s="5">
-        <v>1005</v>
+        <v>40</v>
       </c>
       <c r="E17" s="5">
-        <v>1400</v>
+        <v>500</v>
       </c>
       <c r="F17" s="5">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="G17" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H17" s="5">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="I17" s="5">
-        <v>350</v>
+        <v>160</v>
       </c>
       <c r="J17" s="5">
         <v>0</v>
       </c>
-      <c r="K17" s="5">
-        <v>600</v>
-      </c>
-      <c r="L17" s="5">
-        <v>1000</v>
-      </c>
+      <c r="K17" s="5"/>
+      <c r="L17" s="5"/>
       <c r="M17" s="5"/>
     </row>
     <row r="18" ht="28" customHeight="true" x14ac:dyDescent="0.25">
@@ -1271,7 +1271,7 @@
         <v>38</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C26" s="5">
         <v>2500</v>
@@ -1310,7 +1310,7 @@
         <v>39</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C27" s="5">
         <v>2500</v>
@@ -1349,7 +1349,7 @@
         <v>40</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C28" s="5">
         <v>1500</v>
@@ -1388,7 +1388,7 @@
         <v>41</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C29" s="5">
         <v>2000</v>

</xml_diff>

<commit_message>
[Feat] (Client) Create DynaNest Object By NestBuilder Class
</commit_message>
<xml_diff>
--- a/CharacterStats.xlsx
+++ b/CharacterStats.xlsx
@@ -72,31 +72,31 @@
     <t>Normal</t>
   </si>
   <si>
+    <t>Chicken</t>
+  </si>
+  <si>
     <t>YellowBird</t>
   </si>
   <si>
-    <t>Chicken</t>
+    <t>Frog</t>
   </si>
   <si>
     <t>MushRoom</t>
   </si>
   <si>
-    <t>Frog</t>
+    <t>Kabu</t>
   </si>
   <si>
     <t>PurpleBeatle</t>
   </si>
   <si>
-    <t>Kabu</t>
+    <t>NormalBear</t>
   </si>
   <si>
     <t>BossDyna</t>
   </si>
   <si>
     <t>Boss</t>
-  </si>
-  <si>
-    <t>NormalBear</t>
   </si>
   <si>
     <t>Scary</t>
@@ -852,13 +852,13 @@
         <v>100</v>
       </c>
       <c r="G14" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H14" s="5">
         <v>50</v>
       </c>
       <c r="I14" s="5">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="J14" s="5">
         <v>0</v>
@@ -887,13 +887,13 @@
         <v>100</v>
       </c>
       <c r="G15" s="5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H15" s="5">
         <v>50</v>
       </c>
       <c r="I15" s="5">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="J15" s="5">
         <v>0</v>
@@ -907,73 +907,73 @@
         <v>25</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="C16" s="5">
-        <v>2500</v>
+        <v>200</v>
       </c>
       <c r="D16" s="5">
-        <v>1005</v>
+        <v>40</v>
       </c>
       <c r="E16" s="5">
-        <v>1400</v>
+        <v>500</v>
       </c>
       <c r="F16" s="5">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="G16" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H16" s="5">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="I16" s="5">
-        <v>350</v>
+        <v>160</v>
       </c>
       <c r="J16" s="5">
         <v>0</v>
       </c>
-      <c r="K16" s="5">
-        <v>600</v>
-      </c>
-      <c r="L16" s="5">
-        <v>1000</v>
-      </c>
+      <c r="K16" s="5"/>
+      <c r="L16" s="5"/>
       <c r="M16" s="5"/>
     </row>
     <row r="17" ht="28" customHeight="true" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B17" s="5" t="s">
-        <v>18</v>
-      </c>
       <c r="C17" s="5">
-        <v>200</v>
+        <v>2500</v>
       </c>
       <c r="D17" s="5">
-        <v>40</v>
+        <v>1005</v>
       </c>
       <c r="E17" s="5">
-        <v>500</v>
+        <v>1400</v>
       </c>
       <c r="F17" s="5">
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="G17" s="5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H17" s="5">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="I17" s="5">
-        <v>160</v>
+        <v>350</v>
       </c>
       <c r="J17" s="5">
         <v>0</v>
       </c>
-      <c r="K17" s="5"/>
-      <c r="L17" s="5"/>
+      <c r="K17" s="5">
+        <v>600</v>
+      </c>
+      <c r="L17" s="5">
+        <v>1000</v>
+      </c>
       <c r="M17" s="5"/>
     </row>
     <row r="18" ht="28" customHeight="true" x14ac:dyDescent="0.25">
@@ -1271,7 +1271,7 @@
         <v>38</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C26" s="5">
         <v>2500</v>
@@ -1310,7 +1310,7 @@
         <v>39</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C27" s="5">
         <v>2500</v>
@@ -1349,7 +1349,7 @@
         <v>40</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C28" s="5">
         <v>1500</v>
@@ -1388,7 +1388,7 @@
         <v>41</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C29" s="5">
         <v>2000</v>

</xml_diff>

<commit_message>
[Feat] (Client) Create BossDyna Baby Object By DynaBabyBuilder Class
</commit_message>
<xml_diff>
--- a/CharacterStats.xlsx
+++ b/CharacterStats.xlsx
@@ -72,31 +72,31 @@
     <t>Normal</t>
   </si>
   <si>
+    <t>YellowBird</t>
+  </si>
+  <si>
     <t>Chicken</t>
   </si>
   <si>
-    <t>YellowBird</t>
+    <t>MushRoom</t>
   </si>
   <si>
     <t>Frog</t>
   </si>
   <si>
-    <t>MushRoom</t>
+    <t>PurpleBeatle</t>
   </si>
   <si>
     <t>Kabu</t>
   </si>
   <si>
-    <t>PurpleBeatle</t>
+    <t>BossDyna</t>
+  </si>
+  <si>
+    <t>Boss</t>
   </si>
   <si>
     <t>NormalBear</t>
-  </si>
-  <si>
-    <t>BossDyna</t>
-  </si>
-  <si>
-    <t>Boss</t>
   </si>
   <si>
     <t>Scary</t>
@@ -852,13 +852,13 @@
         <v>100</v>
       </c>
       <c r="G14" s="5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H14" s="5">
         <v>50</v>
       </c>
       <c r="I14" s="5">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="J14" s="5">
         <v>0</v>
@@ -887,13 +887,13 @@
         <v>100</v>
       </c>
       <c r="G15" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H15" s="5">
         <v>50</v>
       </c>
       <c r="I15" s="5">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="J15" s="5">
         <v>0</v>
@@ -907,73 +907,73 @@
         <v>25</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="C16" s="5">
-        <v>200</v>
+        <v>2500</v>
       </c>
       <c r="D16" s="5">
-        <v>40</v>
+        <v>1005</v>
       </c>
       <c r="E16" s="5">
-        <v>500</v>
+        <v>1400</v>
       </c>
       <c r="F16" s="5">
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="G16" s="5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H16" s="5">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="I16" s="5">
-        <v>160</v>
+        <v>350</v>
       </c>
       <c r="J16" s="5">
         <v>0</v>
       </c>
-      <c r="K16" s="5"/>
-      <c r="L16" s="5"/>
+      <c r="K16" s="5">
+        <v>600</v>
+      </c>
+      <c r="L16" s="5">
+        <v>1000</v>
+      </c>
       <c r="M16" s="5"/>
     </row>
     <row r="17" ht="28" customHeight="true" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="C17" s="5">
-        <v>2500</v>
+        <v>200</v>
       </c>
       <c r="D17" s="5">
-        <v>1005</v>
+        <v>40</v>
       </c>
       <c r="E17" s="5">
-        <v>1400</v>
+        <v>500</v>
       </c>
       <c r="F17" s="5">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="G17" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H17" s="5">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="I17" s="5">
-        <v>350</v>
+        <v>160</v>
       </c>
       <c r="J17" s="5">
         <v>0</v>
       </c>
-      <c r="K17" s="5">
-        <v>600</v>
-      </c>
-      <c r="L17" s="5">
-        <v>1000</v>
-      </c>
+      <c r="K17" s="5"/>
+      <c r="L17" s="5"/>
       <c r="M17" s="5"/>
     </row>
     <row r="18" ht="28" customHeight="true" x14ac:dyDescent="0.25">
@@ -1271,7 +1271,7 @@
         <v>38</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C26" s="5">
         <v>2500</v>
@@ -1310,7 +1310,7 @@
         <v>39</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C27" s="5">
         <v>2500</v>
@@ -1349,7 +1349,7 @@
         <v>40</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C28" s="5">
         <v>1500</v>
@@ -1388,7 +1388,7 @@
         <v>41</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C29" s="5">
         <v>2000</v>

</xml_diff>

<commit_message>
[Feat] (Client) Delete All Remaining BossDynaBabies When Boss Dyna Is Destroyed
</commit_message>
<xml_diff>
--- a/CharacterStats.xlsx
+++ b/CharacterStats.xlsx
@@ -72,31 +72,31 @@
     <t>Normal</t>
   </si>
   <si>
+    <t>Chicken</t>
+  </si>
+  <si>
     <t>YellowBird</t>
   </si>
   <si>
-    <t>Chicken</t>
+    <t>Frog</t>
   </si>
   <si>
     <t>MushRoom</t>
   </si>
   <si>
-    <t>Frog</t>
+    <t>Kabu</t>
   </si>
   <si>
     <t>PurpleBeatle</t>
   </si>
   <si>
-    <t>Kabu</t>
+    <t>NormalBear</t>
   </si>
   <si>
     <t>BossDyna</t>
   </si>
   <si>
     <t>Boss</t>
-  </si>
-  <si>
-    <t>NormalBear</t>
   </si>
   <si>
     <t>Scary</t>
@@ -852,13 +852,13 @@
         <v>100</v>
       </c>
       <c r="G14" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H14" s="5">
         <v>50</v>
       </c>
       <c r="I14" s="5">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="J14" s="5">
         <v>0</v>
@@ -887,13 +887,13 @@
         <v>100</v>
       </c>
       <c r="G15" s="5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H15" s="5">
         <v>50</v>
       </c>
       <c r="I15" s="5">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="J15" s="5">
         <v>0</v>
@@ -907,73 +907,73 @@
         <v>25</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="C16" s="5">
-        <v>2500</v>
+        <v>200</v>
       </c>
       <c r="D16" s="5">
-        <v>1005</v>
+        <v>40</v>
       </c>
       <c r="E16" s="5">
-        <v>1400</v>
+        <v>500</v>
       </c>
       <c r="F16" s="5">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="G16" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H16" s="5">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="I16" s="5">
-        <v>350</v>
+        <v>160</v>
       </c>
       <c r="J16" s="5">
         <v>0</v>
       </c>
-      <c r="K16" s="5">
-        <v>600</v>
-      </c>
-      <c r="L16" s="5">
-        <v>1000</v>
-      </c>
+      <c r="K16" s="5"/>
+      <c r="L16" s="5"/>
       <c r="M16" s="5"/>
     </row>
     <row r="17" ht="28" customHeight="true" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B17" s="5" t="s">
-        <v>18</v>
-      </c>
       <c r="C17" s="5">
-        <v>200</v>
+        <v>2500</v>
       </c>
       <c r="D17" s="5">
-        <v>40</v>
+        <v>1005</v>
       </c>
       <c r="E17" s="5">
-        <v>500</v>
+        <v>1400</v>
       </c>
       <c r="F17" s="5">
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="G17" s="5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H17" s="5">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="I17" s="5">
-        <v>160</v>
+        <v>350</v>
       </c>
       <c r="J17" s="5">
         <v>0</v>
       </c>
-      <c r="K17" s="5"/>
-      <c r="L17" s="5"/>
+      <c r="K17" s="5">
+        <v>600</v>
+      </c>
+      <c r="L17" s="5">
+        <v>1000</v>
+      </c>
       <c r="M17" s="5"/>
     </row>
     <row r="18" ht="28" customHeight="true" x14ac:dyDescent="0.25">
@@ -1271,7 +1271,7 @@
         <v>38</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C26" s="5">
         <v>2500</v>
@@ -1310,7 +1310,7 @@
         <v>39</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C27" s="5">
         <v>2500</v>
@@ -1349,7 +1349,7 @@
         <v>40</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C28" s="5">
         <v>1500</v>
@@ -1388,7 +1388,7 @@
         <v>41</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C29" s="5">
         <v>2000</v>

</xml_diff>

<commit_message>
[Feat] (Engine) Create GameObjectManager Class Which Is A Base Class Of Classes That Managers Object ex) Pool, Factory, Builder
</commit_message>
<xml_diff>
--- a/CharacterStats.xlsx
+++ b/CharacterStats.xlsx
@@ -72,31 +72,31 @@
     <t>Normal</t>
   </si>
   <si>
+    <t>YellowBird</t>
+  </si>
+  <si>
     <t>Chicken</t>
   </si>
   <si>
-    <t>YellowBird</t>
+    <t>MushRoom</t>
   </si>
   <si>
     <t>Frog</t>
   </si>
   <si>
-    <t>MushRoom</t>
+    <t>PurpleBeatle</t>
   </si>
   <si>
     <t>Kabu</t>
   </si>
   <si>
-    <t>PurpleBeatle</t>
+    <t>BossDyna</t>
+  </si>
+  <si>
+    <t>Boss</t>
   </si>
   <si>
     <t>NormalBear</t>
-  </si>
-  <si>
-    <t>BossDyna</t>
-  </si>
-  <si>
-    <t>Boss</t>
   </si>
   <si>
     <t>Scary</t>
@@ -852,13 +852,13 @@
         <v>100</v>
       </c>
       <c r="G14" s="5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H14" s="5">
         <v>50</v>
       </c>
       <c r="I14" s="5">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="J14" s="5">
         <v>0</v>
@@ -887,13 +887,13 @@
         <v>100</v>
       </c>
       <c r="G15" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H15" s="5">
         <v>50</v>
       </c>
       <c r="I15" s="5">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="J15" s="5">
         <v>0</v>
@@ -907,73 +907,73 @@
         <v>25</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="C16" s="5">
-        <v>200</v>
+        <v>2500</v>
       </c>
       <c r="D16" s="5">
-        <v>40</v>
+        <v>1005</v>
       </c>
       <c r="E16" s="5">
-        <v>500</v>
+        <v>1400</v>
       </c>
       <c r="F16" s="5">
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="G16" s="5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H16" s="5">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="I16" s="5">
-        <v>160</v>
+        <v>350</v>
       </c>
       <c r="J16" s="5">
         <v>0</v>
       </c>
-      <c r="K16" s="5"/>
-      <c r="L16" s="5"/>
+      <c r="K16" s="5">
+        <v>600</v>
+      </c>
+      <c r="L16" s="5">
+        <v>1000</v>
+      </c>
       <c r="M16" s="5"/>
     </row>
     <row r="17" ht="28" customHeight="true" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="C17" s="5">
-        <v>2500</v>
+        <v>200</v>
       </c>
       <c r="D17" s="5">
-        <v>1005</v>
+        <v>40</v>
       </c>
       <c r="E17" s="5">
-        <v>1400</v>
+        <v>500</v>
       </c>
       <c r="F17" s="5">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="G17" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H17" s="5">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="I17" s="5">
-        <v>350</v>
+        <v>160</v>
       </c>
       <c r="J17" s="5">
         <v>0</v>
       </c>
-      <c r="K17" s="5">
-        <v>600</v>
-      </c>
-      <c r="L17" s="5">
-        <v>1000</v>
-      </c>
+      <c r="K17" s="5"/>
+      <c r="L17" s="5"/>
       <c r="M17" s="5"/>
     </row>
     <row r="18" ht="28" customHeight="true" x14ac:dyDescent="0.25">
@@ -1271,7 +1271,7 @@
         <v>38</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C26" s="5">
         <v>2500</v>
@@ -1310,7 +1310,7 @@
         <v>39</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C27" s="5">
         <v>2500</v>
@@ -1349,7 +1349,7 @@
         <v>40</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C28" s="5">
         <v>1500</v>
@@ -1388,7 +1388,7 @@
         <v>41</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C29" s="5">
         <v>2000</v>

</xml_diff>